<commit_message>
img, some js and pages are added
</commit_message>
<xml_diff>
--- a/database/database.xlsx
+++ b/database/database.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="555" windowWidth="19815" windowHeight="7365"/>
+    <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1224" uniqueCount="458">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="458">
   <si>
     <t>id</t>
   </si>
@@ -1393,24 +1393,23 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -1425,40 +1424,26 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -1746,16 +1731,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:D408"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1769,12 +1758,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
+    <row r="2" spans="1:4">
+      <c r="A2" s="1" t="n">
         <v>1027</v>
       </c>
-      <c r="B2">
-        <v>2899</v>
+      <c r="B2" t="s">
+        <v>4</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
@@ -1783,8 +1772,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
+    <row r="3" spans="1:4">
+      <c r="A3" s="1" t="n">
         <v>1028</v>
       </c>
       <c r="B3" t="s">
@@ -1797,8 +1786,8 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
+    <row r="4" spans="1:4">
+      <c r="A4" s="1" t="n">
         <v>1029</v>
       </c>
       <c r="B4" t="s">
@@ -1811,8 +1800,8 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
+    <row r="5" spans="1:4">
+      <c r="A5" s="1" t="n">
         <v>1030</v>
       </c>
       <c r="B5" t="s">
@@ -1825,8 +1814,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
+    <row r="6" spans="1:4">
+      <c r="A6" s="1" t="n">
         <v>1031</v>
       </c>
       <c r="B6" t="s">
@@ -1839,8 +1828,8 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
+    <row r="7" spans="1:4">
+      <c r="A7" s="1" t="n">
         <v>1032</v>
       </c>
       <c r="B7" t="s">
@@ -1853,8 +1842,8 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
+    <row r="8" spans="1:4">
+      <c r="A8" s="1" t="n">
         <v>1033</v>
       </c>
       <c r="B8" t="s">
@@ -1867,8 +1856,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
+    <row r="9" spans="1:4">
+      <c r="A9" s="1" t="n">
         <v>1034</v>
       </c>
       <c r="B9" t="s">
@@ -1881,8 +1870,8 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
+    <row r="10" spans="1:4">
+      <c r="A10" s="1" t="n">
         <v>1035</v>
       </c>
       <c r="B10" t="s">
@@ -1895,8 +1884,8 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
+    <row r="11" spans="1:4">
+      <c r="A11" s="1" t="n">
         <v>1036</v>
       </c>
       <c r="B11" t="s">
@@ -1909,8 +1898,8 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
+    <row r="12" spans="1:4">
+      <c r="A12" s="1" t="n">
         <v>1037</v>
       </c>
       <c r="B12" t="s">
@@ -1923,8 +1912,8 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
+    <row r="13" spans="1:4">
+      <c r="A13" s="1" t="n">
         <v>1038</v>
       </c>
       <c r="B13" t="s">
@@ -1937,8 +1926,8 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
+    <row r="14" spans="1:4">
+      <c r="A14" s="1" t="n">
         <v>1039</v>
       </c>
       <c r="B14" t="s">
@@ -1951,8 +1940,8 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
+    <row r="15" spans="1:4">
+      <c r="A15" s="1" t="n">
         <v>1040</v>
       </c>
       <c r="B15" t="s">
@@ -1965,8 +1954,8 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
+    <row r="16" spans="1:4">
+      <c r="A16" s="1" t="n">
         <v>1041</v>
       </c>
       <c r="B16" t="s">
@@ -1979,8 +1968,8 @@
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
+    <row r="17" spans="1:4">
+      <c r="A17" s="1" t="n">
         <v>1042</v>
       </c>
       <c r="B17" t="s">
@@ -1993,8 +1982,8 @@
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="1">
+    <row r="18" spans="1:4">
+      <c r="A18" s="1" t="n">
         <v>1043</v>
       </c>
       <c r="B18" t="s">
@@ -2007,8 +1996,8 @@
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
+    <row r="19" spans="1:4">
+      <c r="A19" s="1" t="n">
         <v>1044</v>
       </c>
       <c r="B19" t="s">
@@ -2021,8 +2010,8 @@
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="1">
+    <row r="20" spans="1:4">
+      <c r="A20" s="1" t="n">
         <v>1045</v>
       </c>
       <c r="B20" t="s">
@@ -2035,8 +2024,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="1">
+    <row r="21" spans="1:4">
+      <c r="A21" s="1" t="n">
         <v>1046</v>
       </c>
       <c r="B21" t="s">
@@ -2049,8 +2038,8 @@
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="1">
+    <row r="22" spans="1:4">
+      <c r="A22" s="1" t="n">
         <v>1047</v>
       </c>
       <c r="B22" t="s">
@@ -2063,8 +2052,8 @@
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="1">
+    <row r="23" spans="1:4">
+      <c r="A23" s="1" t="n">
         <v>1048</v>
       </c>
       <c r="B23" t="s">
@@ -2077,8 +2066,8 @@
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="1">
+    <row r="24" spans="1:4">
+      <c r="A24" s="1" t="n">
         <v>1049</v>
       </c>
       <c r="B24" t="s">
@@ -2091,8 +2080,8 @@
         <v>31</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="1">
+    <row r="25" spans="1:4">
+      <c r="A25" s="1" t="n">
         <v>1050</v>
       </c>
       <c r="B25" t="s">
@@ -2105,8 +2094,8 @@
         <v>34</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="1">
+    <row r="26" spans="1:4">
+      <c r="A26" s="1" t="n">
         <v>1051</v>
       </c>
       <c r="B26" t="s">
@@ -2119,8 +2108,8 @@
         <v>12</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="1">
+    <row r="27" spans="1:4">
+      <c r="A27" s="1" t="n">
         <v>1052</v>
       </c>
       <c r="B27" t="s">
@@ -2133,8 +2122,8 @@
         <v>16</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="1">
+    <row r="28" spans="1:4">
+      <c r="A28" s="1" t="n">
         <v>1053</v>
       </c>
       <c r="B28" t="s">
@@ -2147,8 +2136,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="1">
+    <row r="29" spans="1:4">
+      <c r="A29" s="1" t="n">
         <v>1054</v>
       </c>
       <c r="B29" t="s">
@@ -2161,8 +2150,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="1">
+    <row r="30" spans="1:4">
+      <c r="A30" s="1" t="n">
         <v>1055</v>
       </c>
       <c r="B30" t="s">
@@ -2175,8 +2164,8 @@
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="1">
+    <row r="31" spans="1:4">
+      <c r="A31" s="1" t="n">
         <v>1056</v>
       </c>
       <c r="B31" t="s">
@@ -2189,8 +2178,8 @@
         <v>12</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="1">
+    <row r="32" spans="1:4">
+      <c r="A32" s="1" t="n">
         <v>1057</v>
       </c>
       <c r="B32" t="s">
@@ -2203,8 +2192,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="1">
+    <row r="33" spans="1:4">
+      <c r="A33" s="1" t="n">
         <v>1058</v>
       </c>
       <c r="B33" t="s">
@@ -2217,8 +2206,8 @@
         <v>14</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="1">
+    <row r="34" spans="1:4">
+      <c r="A34" s="1" t="n">
         <v>1059</v>
       </c>
       <c r="B34" t="s">
@@ -2231,8 +2220,8 @@
         <v>16</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="1">
+    <row r="35" spans="1:4">
+      <c r="A35" s="1" t="n">
         <v>1060</v>
       </c>
       <c r="B35" t="s">
@@ -2245,8 +2234,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="1">
+    <row r="36" spans="1:4">
+      <c r="A36" s="1" t="n">
         <v>1061</v>
       </c>
       <c r="B36" t="s">
@@ -2259,8 +2248,8 @@
         <v>9</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="1">
+    <row r="37" spans="1:4">
+      <c r="A37" s="1" t="n">
         <v>1062</v>
       </c>
       <c r="B37" t="s">
@@ -2273,8 +2262,8 @@
         <v>19</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="1">
+    <row r="38" spans="1:4">
+      <c r="A38" s="1" t="n">
         <v>1063</v>
       </c>
       <c r="B38" t="s">
@@ -2287,8 +2276,8 @@
         <v>19</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="1">
+    <row r="39" spans="1:4">
+      <c r="A39" s="1" t="n">
         <v>1064</v>
       </c>
       <c r="B39" t="s">
@@ -2301,8 +2290,8 @@
         <v>20</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="1">
+    <row r="40" spans="1:4">
+      <c r="A40" s="1" t="n">
         <v>1065</v>
       </c>
       <c r="B40" t="s">
@@ -2315,8 +2304,8 @@
         <v>20</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="1">
+    <row r="41" spans="1:4">
+      <c r="A41" s="1" t="n">
         <v>1066</v>
       </c>
       <c r="B41" t="s">
@@ -2329,8 +2318,8 @@
         <v>21</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="1">
+    <row r="42" spans="1:4">
+      <c r="A42" s="1" t="n">
         <v>1067</v>
       </c>
       <c r="B42" t="s">
@@ -2343,8 +2332,8 @@
         <v>22</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="1">
+    <row r="43" spans="1:4">
+      <c r="A43" s="1" t="n">
         <v>1068</v>
       </c>
       <c r="B43" t="s">
@@ -2357,8 +2346,8 @@
         <v>23</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="1">
+    <row r="44" spans="1:4">
+      <c r="A44" s="1" t="n">
         <v>1069</v>
       </c>
       <c r="B44" t="s">
@@ -2371,8 +2360,8 @@
         <v>24</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="1">
+    <row r="45" spans="1:4">
+      <c r="A45" s="1" t="n">
         <v>1070</v>
       </c>
       <c r="B45" t="s">
@@ -2385,8 +2374,8 @@
         <v>21</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="1">
+    <row r="46" spans="1:4">
+      <c r="A46" s="1" t="n">
         <v>1071</v>
       </c>
       <c r="B46" t="s">
@@ -2399,8 +2388,8 @@
         <v>22</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="1">
+    <row r="47" spans="1:4">
+      <c r="A47" s="1" t="n">
         <v>1072</v>
       </c>
       <c r="B47" t="s">
@@ -2413,8 +2402,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="1">
+    <row r="48" spans="1:4">
+      <c r="A48" s="1" t="n">
         <v>1073</v>
       </c>
       <c r="B48" t="s">
@@ -2427,8 +2416,8 @@
         <v>26</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="1">
+    <row r="49" spans="1:4">
+      <c r="A49" s="1" t="n">
         <v>1074</v>
       </c>
       <c r="B49" t="s">
@@ -2441,8 +2430,8 @@
         <v>27</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="1">
+    <row r="50" spans="1:4">
+      <c r="A50" s="1" t="n">
         <v>1075</v>
       </c>
       <c r="B50" t="s">
@@ -2455,8 +2444,8 @@
         <v>28</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="1">
+    <row r="51" spans="1:4">
+      <c r="A51" s="1" t="n">
         <v>1076</v>
       </c>
       <c r="B51" t="s">
@@ -2469,8 +2458,8 @@
         <v>31</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="1">
+    <row r="52" spans="1:4">
+      <c r="A52" s="1" t="n">
         <v>1077</v>
       </c>
       <c r="B52" t="s">
@@ -2483,8 +2472,8 @@
         <v>34</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="1">
+    <row r="53" spans="1:4">
+      <c r="A53" s="1" t="n">
         <v>1078</v>
       </c>
       <c r="B53" t="s">
@@ -2497,8 +2486,8 @@
         <v>12</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="1">
+    <row r="54" spans="1:4">
+      <c r="A54" s="1" t="n">
         <v>1079</v>
       </c>
       <c r="B54" t="s">
@@ -2511,8 +2500,8 @@
         <v>16</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="1">
+    <row r="55" spans="1:4">
+      <c r="A55" s="1" t="n">
         <v>1080</v>
       </c>
       <c r="B55" t="s">
@@ -2525,8 +2514,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="1">
+    <row r="56" spans="1:4">
+      <c r="A56" s="1" t="n">
         <v>1081</v>
       </c>
       <c r="B56" t="s">
@@ -2539,8 +2528,8 @@
         <v>40</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="1">
+    <row r="57" spans="1:4">
+      <c r="A57" s="1" t="n">
         <v>1082</v>
       </c>
       <c r="B57" t="s">
@@ -2553,8 +2542,8 @@
         <v>41</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="1">
+    <row r="58" spans="1:4">
+      <c r="A58" s="1" t="n">
         <v>1083</v>
       </c>
       <c r="B58" t="s">
@@ -2567,8 +2556,8 @@
         <v>43</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="1">
+    <row r="59" spans="1:4">
+      <c r="A59" s="1" t="n">
         <v>1084</v>
       </c>
       <c r="B59" t="s">
@@ -2581,8 +2570,8 @@
         <v>45</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="1">
+    <row r="60" spans="1:4">
+      <c r="A60" s="1" t="n">
         <v>1085</v>
       </c>
       <c r="B60" t="s">
@@ -2595,8 +2584,8 @@
         <v>47</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="1">
+    <row r="61" spans="1:4">
+      <c r="A61" s="1" t="n">
         <v>1086</v>
       </c>
       <c r="B61" t="s">
@@ -2609,8 +2598,8 @@
         <v>40</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="1">
+    <row r="62" spans="1:4">
+      <c r="A62" s="1" t="n">
         <v>1087</v>
       </c>
       <c r="B62" t="s">
@@ -2623,8 +2612,8 @@
         <v>50</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="1">
+    <row r="63" spans="1:4">
+      <c r="A63" s="1" t="n">
         <v>1088</v>
       </c>
       <c r="B63" t="s">
@@ -2637,8 +2626,8 @@
         <v>51</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="1">
+    <row r="64" spans="1:4">
+      <c r="A64" s="1" t="n">
         <v>1089</v>
       </c>
       <c r="B64" t="s">
@@ -2651,8 +2640,8 @@
         <v>52</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="1">
+    <row r="65" spans="1:4">
+      <c r="A65" s="1" t="n">
         <v>1090</v>
       </c>
       <c r="B65" t="s">
@@ -2665,8 +2654,8 @@
         <v>53</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="1">
+    <row r="66" spans="1:4">
+      <c r="A66" s="1" t="n">
         <v>1091</v>
       </c>
       <c r="B66" t="s">
@@ -2679,8 +2668,8 @@
         <v>54</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="1">
+    <row r="67" spans="1:4">
+      <c r="A67" s="1" t="n">
         <v>1092</v>
       </c>
       <c r="B67" t="s">
@@ -2693,8 +2682,8 @@
         <v>56</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="1">
+    <row r="68" spans="1:4">
+      <c r="A68" s="1" t="n">
         <v>1093</v>
       </c>
       <c r="B68" t="s">
@@ -2707,8 +2696,8 @@
         <v>58</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="1">
+    <row r="69" spans="1:4">
+      <c r="A69" s="1" t="n">
         <v>1094</v>
       </c>
       <c r="B69" t="s">
@@ -2721,8 +2710,8 @@
         <v>60</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" s="1">
+    <row r="70" spans="1:4">
+      <c r="A70" s="1" t="n">
         <v>1095</v>
       </c>
       <c r="B70" t="s">
@@ -2735,8 +2724,8 @@
         <v>61</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="1">
+    <row r="71" spans="1:4">
+      <c r="A71" s="1" t="n">
         <v>1096</v>
       </c>
       <c r="B71" t="s">
@@ -2749,8 +2738,8 @@
         <v>62</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="1">
+    <row r="72" spans="1:4">
+      <c r="A72" s="1" t="n">
         <v>1097</v>
       </c>
       <c r="B72" t="s">
@@ -2763,8 +2752,8 @@
         <v>63</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="1">
+    <row r="73" spans="1:4">
+      <c r="A73" s="1" t="n">
         <v>1098</v>
       </c>
       <c r="B73" t="s">
@@ -2777,8 +2766,8 @@
         <v>64</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" s="1">
+    <row r="74" spans="1:4">
+      <c r="A74" s="1" t="n">
         <v>1099</v>
       </c>
       <c r="B74" t="s">
@@ -2791,8 +2780,8 @@
         <v>65</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="1">
+    <row r="75" spans="1:4">
+      <c r="A75" s="1" t="n">
         <v>1100</v>
       </c>
       <c r="B75" t="s">
@@ -2805,8 +2794,8 @@
         <v>66</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="1">
+    <row r="76" spans="1:4">
+      <c r="A76" s="1" t="n">
         <v>1101</v>
       </c>
       <c r="B76" t="s">
@@ -2819,8 +2808,8 @@
         <v>67</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="1">
+    <row r="77" spans="1:4">
+      <c r="A77" s="1" t="n">
         <v>1102</v>
       </c>
       <c r="B77" t="s">
@@ -2833,8 +2822,8 @@
         <v>69</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="1">
+    <row r="78" spans="1:4">
+      <c r="A78" s="1" t="n">
         <v>1103</v>
       </c>
       <c r="B78" t="s">
@@ -2847,8 +2836,8 @@
         <v>71</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="1">
+    <row r="79" spans="1:4">
+      <c r="A79" s="1" t="n">
         <v>1104</v>
       </c>
       <c r="B79" t="s">
@@ -2861,8 +2850,8 @@
         <v>73</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="1">
+    <row r="80" spans="1:4">
+      <c r="A80" s="1" t="n">
         <v>1105</v>
       </c>
       <c r="B80" t="s">
@@ -2875,8 +2864,8 @@
         <v>75</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" s="1">
+    <row r="81" spans="1:4">
+      <c r="A81" s="1" t="n">
         <v>1106</v>
       </c>
       <c r="B81" t="s">
@@ -2889,8 +2878,8 @@
         <v>77</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" s="1">
+    <row r="82" spans="1:4">
+      <c r="A82" s="1" t="n">
         <v>1107</v>
       </c>
       <c r="B82" t="s">
@@ -2903,8 +2892,8 @@
         <v>79</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83" s="1">
+    <row r="83" spans="1:4">
+      <c r="A83" s="1" t="n">
         <v>1108</v>
       </c>
       <c r="B83" t="s">
@@ -2917,8 +2906,8 @@
         <v>80</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84" s="1">
+    <row r="84" spans="1:4">
+      <c r="A84" s="1" t="n">
         <v>1109</v>
       </c>
       <c r="B84" t="s">
@@ -2931,8 +2920,8 @@
         <v>79</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85" s="1">
+    <row r="85" spans="1:4">
+      <c r="A85" s="1" t="n">
         <v>1110</v>
       </c>
       <c r="B85" t="s">
@@ -2945,8 +2934,8 @@
         <v>80</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A86" s="1">
+    <row r="86" spans="1:4">
+      <c r="A86" s="1" t="n">
         <v>1111</v>
       </c>
       <c r="B86" t="s">
@@ -2959,8 +2948,8 @@
         <v>83</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A87" s="1">
+    <row r="87" spans="1:4">
+      <c r="A87" s="1" t="n">
         <v>1112</v>
       </c>
       <c r="B87" t="s">
@@ -2973,8 +2962,8 @@
         <v>83</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88" s="1">
+    <row r="88" spans="1:4">
+      <c r="A88" s="1" t="n">
         <v>1113</v>
       </c>
       <c r="B88" t="s">
@@ -2987,8 +2976,8 @@
         <v>86</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A89" s="1">
+    <row r="89" spans="1:4">
+      <c r="A89" s="1" t="n">
         <v>1114</v>
       </c>
       <c r="B89" t="s">
@@ -3001,8 +2990,8 @@
         <v>86</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A90" s="1">
+    <row r="90" spans="1:4">
+      <c r="A90" s="1" t="n">
         <v>1115</v>
       </c>
       <c r="B90" t="s">
@@ -3015,8 +3004,8 @@
         <v>89</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A91" s="1">
+    <row r="91" spans="1:4">
+      <c r="A91" s="1" t="n">
         <v>1116</v>
       </c>
       <c r="B91" t="s">
@@ -3029,8 +3018,8 @@
         <v>89</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A92" s="1">
+    <row r="92" spans="1:4">
+      <c r="A92" s="1" t="n">
         <v>1117</v>
       </c>
       <c r="B92" t="s">
@@ -3043,8 +3032,8 @@
         <v>89</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A93" s="1">
+    <row r="93" spans="1:4">
+      <c r="A93" s="1" t="n">
         <v>1118</v>
       </c>
       <c r="B93" t="s">
@@ -3057,8 +3046,8 @@
         <v>93</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A94" s="1">
+    <row r="94" spans="1:4">
+      <c r="A94" s="1" t="n">
         <v>1119</v>
       </c>
       <c r="B94" t="s">
@@ -3071,8 +3060,8 @@
         <v>94</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A95" s="1">
+    <row r="95" spans="1:4">
+      <c r="A95" s="1" t="n">
         <v>1120</v>
       </c>
       <c r="B95" t="s">
@@ -3085,8 +3074,8 @@
         <v>94</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A96" s="1">
+    <row r="96" spans="1:4">
+      <c r="A96" s="1" t="n">
         <v>1121</v>
       </c>
       <c r="B96" t="s">
@@ -3099,8 +3088,8 @@
         <v>96</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A97" s="1">
+    <row r="97" spans="1:4">
+      <c r="A97" s="1" t="n">
         <v>1122</v>
       </c>
       <c r="B97" t="s">
@@ -3113,8 +3102,8 @@
         <v>97</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A98" s="1">
+    <row r="98" spans="1:4">
+      <c r="A98" s="1" t="n">
         <v>1123</v>
       </c>
       <c r="B98" t="s">
@@ -3127,8 +3116,8 @@
         <v>99</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A99" s="1">
+    <row r="99" spans="1:4">
+      <c r="A99" s="1" t="n">
         <v>1124</v>
       </c>
       <c r="B99" t="s">
@@ -3141,8 +3130,8 @@
         <v>101</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A100" s="1">
+    <row r="100" spans="1:4">
+      <c r="A100" s="1" t="n">
         <v>1125</v>
       </c>
       <c r="B100" t="s">
@@ -3155,8 +3144,8 @@
         <v>103</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A101" s="1">
+    <row r="101" spans="1:4">
+      <c r="A101" s="1" t="n">
         <v>1126</v>
       </c>
       <c r="B101" t="s">
@@ -3169,8 +3158,8 @@
         <v>105</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A102" s="1">
+    <row r="102" spans="1:4">
+      <c r="A102" s="1" t="n">
         <v>1127</v>
       </c>
       <c r="B102" t="s">
@@ -3183,8 +3172,8 @@
         <v>107</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A103" s="1">
+    <row r="103" spans="1:4">
+      <c r="A103" s="1" t="n">
         <v>1128</v>
       </c>
       <c r="B103" t="s">
@@ -3197,8 +3186,8 @@
         <v>108</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A104" s="1">
+    <row r="104" spans="1:4">
+      <c r="A104" s="1" t="n">
         <v>1129</v>
       </c>
       <c r="B104" t="s">
@@ -3211,8 +3200,8 @@
         <v>108</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A105" s="1">
+    <row r="105" spans="1:4">
+      <c r="A105" s="1" t="n">
         <v>1130</v>
       </c>
       <c r="B105" t="s">
@@ -3225,8 +3214,8 @@
         <v>108</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A106" s="1">
+    <row r="106" spans="1:4">
+      <c r="A106" s="1" t="n">
         <v>1131</v>
       </c>
       <c r="B106" t="s">
@@ -3239,8 +3228,8 @@
         <v>112</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A107" s="1">
+    <row r="107" spans="1:4">
+      <c r="A107" s="1" t="n">
         <v>1132</v>
       </c>
       <c r="B107" t="s">
@@ -3253,8 +3242,8 @@
         <v>113</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A108" s="1">
+    <row r="108" spans="1:4">
+      <c r="A108" s="1" t="n">
         <v>1133</v>
       </c>
       <c r="B108" t="s">
@@ -3267,8 +3256,8 @@
         <v>116</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A109" s="1">
+    <row r="109" spans="1:4">
+      <c r="A109" s="1" t="n">
         <v>1134</v>
       </c>
       <c r="B109" t="s">
@@ -3281,8 +3270,8 @@
         <v>116</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A110" s="1">
+    <row r="110" spans="1:4">
+      <c r="A110" s="1" t="n">
         <v>1135</v>
       </c>
       <c r="B110" t="s">
@@ -3295,8 +3284,8 @@
         <v>119</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A111" s="1">
+    <row r="111" spans="1:4">
+      <c r="A111" s="1" t="n">
         <v>1136</v>
       </c>
       <c r="B111" t="s">
@@ -3309,8 +3298,8 @@
         <v>122</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A112" s="1">
+    <row r="112" spans="1:4">
+      <c r="A112" s="1" t="n">
         <v>1137</v>
       </c>
       <c r="B112" t="s">
@@ -3323,8 +3312,8 @@
         <v>122</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A113" s="1">
+    <row r="113" spans="1:4">
+      <c r="A113" s="1" t="n">
         <v>1138</v>
       </c>
       <c r="B113" t="s">
@@ -3337,8 +3326,8 @@
         <v>126</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A114" s="1">
+    <row r="114" spans="1:4">
+      <c r="A114" s="1" t="n">
         <v>1139</v>
       </c>
       <c r="B114" t="s">
@@ -3351,8 +3340,8 @@
         <v>126</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A115" s="1">
+    <row r="115" spans="1:4">
+      <c r="A115" s="1" t="n">
         <v>1140</v>
       </c>
       <c r="B115" t="s">
@@ -3365,8 +3354,8 @@
         <v>126</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A116" s="1">
+    <row r="116" spans="1:4">
+      <c r="A116" s="1" t="n">
         <v>1141</v>
       </c>
       <c r="B116" t="s">
@@ -3379,8 +3368,8 @@
         <v>126</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A117" s="1">
+    <row r="117" spans="1:4">
+      <c r="A117" s="1" t="n">
         <v>1142</v>
       </c>
       <c r="B117" t="s">
@@ -3393,8 +3382,8 @@
         <v>116</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A118" s="1">
+    <row r="118" spans="1:4">
+      <c r="A118" s="1" t="n">
         <v>1143</v>
       </c>
       <c r="B118" t="s">
@@ -3407,8 +3396,8 @@
         <v>116</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A119" s="1">
+    <row r="119" spans="1:4">
+      <c r="A119" s="1" t="n">
         <v>1144</v>
       </c>
       <c r="B119" t="s">
@@ -3421,8 +3410,8 @@
         <v>116</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A120" s="1">
+    <row r="120" spans="1:4">
+      <c r="A120" s="1" t="n">
         <v>1145</v>
       </c>
       <c r="B120" t="s">
@@ -3435,8 +3424,8 @@
         <v>116</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A121" s="1">
+    <row r="121" spans="1:4">
+      <c r="A121" s="1" t="n">
         <v>1146</v>
       </c>
       <c r="B121" t="s">
@@ -3449,8 +3438,8 @@
         <v>133</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A122" s="1">
+    <row r="122" spans="1:4">
+      <c r="A122" s="1" t="n">
         <v>1147</v>
       </c>
       <c r="B122" t="s">
@@ -3463,8 +3452,8 @@
         <v>135</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A123" s="1">
+    <row r="123" spans="1:4">
+      <c r="A123" s="1" t="n">
         <v>1148</v>
       </c>
       <c r="B123" t="s">
@@ -3477,8 +3466,8 @@
         <v>135</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A124" s="1">
+    <row r="124" spans="1:4">
+      <c r="A124" s="1" t="n">
         <v>1149</v>
       </c>
       <c r="B124" t="s">
@@ -3491,8 +3480,8 @@
         <v>135</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A125" s="1">
+    <row r="125" spans="1:4">
+      <c r="A125" s="1" t="n">
         <v>1150</v>
       </c>
       <c r="B125" t="s">
@@ -3505,8 +3494,8 @@
         <v>139</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A126" s="1">
+    <row r="126" spans="1:4">
+      <c r="A126" s="1" t="n">
         <v>1151</v>
       </c>
       <c r="B126" t="s">
@@ -3519,8 +3508,8 @@
         <v>141</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A127" s="1">
+    <row r="127" spans="1:4">
+      <c r="A127" s="1" t="n">
         <v>1152</v>
       </c>
       <c r="B127" t="s">
@@ -3533,8 +3522,8 @@
         <v>142</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A128" s="1">
+    <row r="128" spans="1:4">
+      <c r="A128" s="1" t="n">
         <v>1153</v>
       </c>
       <c r="B128" t="s">
@@ -3547,8 +3536,8 @@
         <v>141</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A129" s="1">
+    <row r="129" spans="1:4">
+      <c r="A129" s="1" t="n">
         <v>1154</v>
       </c>
       <c r="B129" t="s">
@@ -3561,8 +3550,8 @@
         <v>144</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A130" s="1">
+    <row r="130" spans="1:4">
+      <c r="A130" s="1" t="n">
         <v>1155</v>
       </c>
       <c r="B130" t="s">
@@ -3575,8 +3564,8 @@
         <v>144</v>
       </c>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A131" s="1">
+    <row r="131" spans="1:4">
+      <c r="A131" s="1" t="n">
         <v>1156</v>
       </c>
       <c r="B131" t="s">
@@ -3589,8 +3578,8 @@
         <v>144</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A132" s="1">
+    <row r="132" spans="1:4">
+      <c r="A132" s="1" t="n">
         <v>1157</v>
       </c>
       <c r="B132" t="s">
@@ -3603,8 +3592,8 @@
         <v>144</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A133" s="1">
+    <row r="133" spans="1:4">
+      <c r="A133" s="1" t="n">
         <v>1158</v>
       </c>
       <c r="B133" t="s">
@@ -3617,8 +3606,8 @@
         <v>148</v>
       </c>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A134" s="1">
+    <row r="134" spans="1:4">
+      <c r="A134" s="1" t="n">
         <v>1159</v>
       </c>
       <c r="B134" t="s">
@@ -3631,8 +3620,8 @@
         <v>150</v>
       </c>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A135" s="1">
+    <row r="135" spans="1:4">
+      <c r="A135" s="1" t="n">
         <v>1160</v>
       </c>
       <c r="B135" t="s">
@@ -3645,8 +3634,8 @@
         <v>151</v>
       </c>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A136" s="1">
+    <row r="136" spans="1:4">
+      <c r="A136" s="1" t="n">
         <v>1161</v>
       </c>
       <c r="B136" t="s">
@@ -3659,8 +3648,8 @@
         <v>148</v>
       </c>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A137" s="1">
+    <row r="137" spans="1:4">
+      <c r="A137" s="1" t="n">
         <v>1162</v>
       </c>
       <c r="B137" t="s">
@@ -3673,8 +3662,8 @@
         <v>150</v>
       </c>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A138" s="1">
+    <row r="138" spans="1:4">
+      <c r="A138" s="1" t="n">
         <v>1163</v>
       </c>
       <c r="B138" t="s">
@@ -3687,8 +3676,8 @@
         <v>151</v>
       </c>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A139" s="1">
+    <row r="139" spans="1:4">
+      <c r="A139" s="1" t="n">
         <v>1164</v>
       </c>
       <c r="B139" t="s">
@@ -3701,8 +3690,8 @@
         <v>154</v>
       </c>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A140" s="1">
+    <row r="140" spans="1:4">
+      <c r="A140" s="1" t="n">
         <v>1165</v>
       </c>
       <c r="B140" t="s">
@@ -3715,8 +3704,8 @@
         <v>156</v>
       </c>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A141" s="1">
+    <row r="141" spans="1:4">
+      <c r="A141" s="1" t="n">
         <v>1166</v>
       </c>
       <c r="B141" t="s">
@@ -3729,8 +3718,8 @@
         <v>158</v>
       </c>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A142" s="1">
+    <row r="142" spans="1:4">
+      <c r="A142" s="1" t="n">
         <v>1167</v>
       </c>
       <c r="B142" t="s">
@@ -3743,8 +3732,8 @@
         <v>160</v>
       </c>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A143" s="1">
+    <row r="143" spans="1:4">
+      <c r="A143" s="1" t="n">
         <v>1168</v>
       </c>
       <c r="B143" t="s">
@@ -3757,8 +3746,8 @@
         <v>148</v>
       </c>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A144" s="1">
+    <row r="144" spans="1:4">
+      <c r="A144" s="1" t="n">
         <v>1169</v>
       </c>
       <c r="B144" t="s">
@@ -3771,8 +3760,8 @@
         <v>150</v>
       </c>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A145" s="1">
+    <row r="145" spans="1:4">
+      <c r="A145" s="1" t="n">
         <v>1170</v>
       </c>
       <c r="B145" t="s">
@@ -3785,8 +3774,8 @@
         <v>151</v>
       </c>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A146" s="1">
+    <row r="146" spans="1:4">
+      <c r="A146" s="1" t="n">
         <v>1171</v>
       </c>
       <c r="B146" t="s">
@@ -3799,8 +3788,8 @@
         <v>148</v>
       </c>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A147" s="1">
+    <row r="147" spans="1:4">
+      <c r="A147" s="1" t="n">
         <v>1172</v>
       </c>
       <c r="B147" t="s">
@@ -3813,8 +3802,8 @@
         <v>150</v>
       </c>
     </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A148" s="1">
+    <row r="148" spans="1:4">
+      <c r="A148" s="1" t="n">
         <v>1173</v>
       </c>
       <c r="B148" t="s">
@@ -3827,8 +3816,8 @@
         <v>151</v>
       </c>
     </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A149" s="1">
+    <row r="149" spans="1:4">
+      <c r="A149" s="1" t="n">
         <v>1174</v>
       </c>
       <c r="B149" t="s">
@@ -3841,8 +3830,8 @@
         <v>148</v>
       </c>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A150" s="1">
+    <row r="150" spans="1:4">
+      <c r="A150" s="1" t="n">
         <v>1175</v>
       </c>
       <c r="B150" t="s">
@@ -3855,8 +3844,8 @@
         <v>150</v>
       </c>
     </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A151" s="1">
+    <row r="151" spans="1:4">
+      <c r="A151" s="1" t="n">
         <v>1176</v>
       </c>
       <c r="B151" t="s">
@@ -3869,8 +3858,8 @@
         <v>151</v>
       </c>
     </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A152" s="1">
+    <row r="152" spans="1:4">
+      <c r="A152" s="1" t="n">
         <v>1177</v>
       </c>
       <c r="B152" t="s">
@@ -3883,8 +3872,8 @@
         <v>148</v>
       </c>
     </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A153" s="1">
+    <row r="153" spans="1:4">
+      <c r="A153" s="1" t="n">
         <v>1178</v>
       </c>
       <c r="B153" t="s">
@@ -3897,8 +3886,8 @@
         <v>150</v>
       </c>
     </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A154" s="1">
+    <row r="154" spans="1:4">
+      <c r="A154" s="1" t="n">
         <v>1179</v>
       </c>
       <c r="B154" t="s">
@@ -3911,8 +3900,8 @@
         <v>151</v>
       </c>
     </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A155" s="1">
+    <row r="155" spans="1:4">
+      <c r="A155" s="1" t="n">
         <v>1180</v>
       </c>
       <c r="B155" t="s">
@@ -3925,8 +3914,8 @@
         <v>167</v>
       </c>
     </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A156" s="1">
+    <row r="156" spans="1:4">
+      <c r="A156" s="1" t="n">
         <v>1181</v>
       </c>
       <c r="B156" t="s">
@@ -3939,8 +3928,8 @@
         <v>169</v>
       </c>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A157" s="1">
+    <row r="157" spans="1:4">
+      <c r="A157" s="1" t="n">
         <v>1182</v>
       </c>
       <c r="B157" t="s">
@@ -3953,8 +3942,8 @@
         <v>170</v>
       </c>
     </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A158" s="1">
+    <row r="158" spans="1:4">
+      <c r="A158" s="1" t="n">
         <v>1183</v>
       </c>
       <c r="B158" t="s">
@@ -3967,8 +3956,8 @@
         <v>170</v>
       </c>
     </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A159" s="1">
+    <row r="159" spans="1:4">
+      <c r="A159" s="1" t="n">
         <v>1184</v>
       </c>
       <c r="B159" t="s">
@@ -3981,8 +3970,8 @@
         <v>173</v>
       </c>
     </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A160" s="1">
+    <row r="160" spans="1:4">
+      <c r="A160" s="1" t="n">
         <v>1185</v>
       </c>
       <c r="B160" t="s">
@@ -3995,8 +3984,8 @@
         <v>170</v>
       </c>
     </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A161" s="1">
+    <row r="161" spans="1:4">
+      <c r="A161" s="1" t="n">
         <v>1186</v>
       </c>
       <c r="B161" t="s">
@@ -4009,8 +3998,8 @@
         <v>175</v>
       </c>
     </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A162" s="1">
+    <row r="162" spans="1:4">
+      <c r="A162" s="1" t="n">
         <v>1187</v>
       </c>
       <c r="B162" t="s">
@@ -4023,8 +4012,8 @@
         <v>177</v>
       </c>
     </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A163" s="1">
+    <row r="163" spans="1:4">
+      <c r="A163" s="1" t="n">
         <v>1188</v>
       </c>
       <c r="B163" t="s">
@@ -4037,8 +4026,8 @@
         <v>178</v>
       </c>
     </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A164" s="1">
+    <row r="164" spans="1:4">
+      <c r="A164" s="1" t="n">
         <v>1189</v>
       </c>
       <c r="B164" t="s">
@@ -4051,8 +4040,8 @@
         <v>179</v>
       </c>
     </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A165" s="1">
+    <row r="165" spans="1:4">
+      <c r="A165" s="1" t="n">
         <v>1190</v>
       </c>
       <c r="B165" t="s">
@@ -4065,8 +4054,8 @@
         <v>180</v>
       </c>
     </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A166" s="1">
+    <row r="166" spans="1:4">
+      <c r="A166" s="1" t="n">
         <v>1191</v>
       </c>
       <c r="B166" t="s">
@@ -4079,8 +4068,8 @@
         <v>182</v>
       </c>
     </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A167" s="1">
+    <row r="167" spans="1:4">
+      <c r="A167" s="1" t="n">
         <v>1192</v>
       </c>
       <c r="B167" t="s">
@@ -4093,8 +4082,8 @@
         <v>182</v>
       </c>
     </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A168" s="1">
+    <row r="168" spans="1:4">
+      <c r="A168" s="1" t="n">
         <v>1193</v>
       </c>
       <c r="B168" t="s">
@@ -4107,8 +4096,8 @@
         <v>182</v>
       </c>
     </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A169" s="1">
+    <row r="169" spans="1:4">
+      <c r="A169" s="1" t="n">
         <v>1194</v>
       </c>
       <c r="B169" t="s">
@@ -4121,8 +4110,8 @@
         <v>184</v>
       </c>
     </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A170" s="1">
+    <row r="170" spans="1:4">
+      <c r="A170" s="1" t="n">
         <v>1195</v>
       </c>
       <c r="B170" t="s">
@@ -4135,8 +4124,8 @@
         <v>185</v>
       </c>
     </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A171" s="1">
+    <row r="171" spans="1:4">
+      <c r="A171" s="1" t="n">
         <v>1196</v>
       </c>
       <c r="B171" t="s">
@@ -4149,8 +4138,8 @@
         <v>187</v>
       </c>
     </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A172" s="1">
+    <row r="172" spans="1:4">
+      <c r="A172" s="1" t="n">
         <v>1197</v>
       </c>
       <c r="B172" t="s">
@@ -4163,8 +4152,8 @@
         <v>188</v>
       </c>
     </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A173" s="1">
+    <row r="173" spans="1:4">
+      <c r="A173" s="1" t="n">
         <v>1198</v>
       </c>
       <c r="B173" t="s">
@@ -4177,8 +4166,8 @@
         <v>189</v>
       </c>
     </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A174" s="1">
+    <row r="174" spans="1:4">
+      <c r="A174" s="1" t="n">
         <v>1199</v>
       </c>
       <c r="B174" t="s">
@@ -4191,8 +4180,8 @@
         <v>188</v>
       </c>
     </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A175" s="1">
+    <row r="175" spans="1:4">
+      <c r="A175" s="1" t="n">
         <v>1200</v>
       </c>
       <c r="B175" t="s">
@@ -4205,8 +4194,8 @@
         <v>190</v>
       </c>
     </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A176" s="1">
+    <row r="176" spans="1:4">
+      <c r="A176" s="1" t="n">
         <v>1201</v>
       </c>
       <c r="B176" t="s">
@@ -4219,8 +4208,8 @@
         <v>192</v>
       </c>
     </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A177" s="1">
+    <row r="177" spans="1:4">
+      <c r="A177" s="1" t="n">
         <v>1202</v>
       </c>
       <c r="B177" t="s">
@@ -4233,8 +4222,8 @@
         <v>194</v>
       </c>
     </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A178" s="1">
+    <row r="178" spans="1:4">
+      <c r="A178" s="1" t="n">
         <v>1203</v>
       </c>
       <c r="B178" t="s">
@@ -4247,8 +4236,8 @@
         <v>196</v>
       </c>
     </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A179" s="1">
+    <row r="179" spans="1:4">
+      <c r="A179" s="1" t="n">
         <v>1204</v>
       </c>
       <c r="B179" t="s">
@@ -4261,8 +4250,8 @@
         <v>198</v>
       </c>
     </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A180" s="1">
+    <row r="180" spans="1:4">
+      <c r="A180" s="1" t="n">
         <v>1205</v>
       </c>
       <c r="B180" t="s">
@@ -4275,8 +4264,8 @@
         <v>200</v>
       </c>
     </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A181" s="1">
+    <row r="181" spans="1:4">
+      <c r="A181" s="1" t="n">
         <v>1206</v>
       </c>
       <c r="B181" t="s">
@@ -4289,8 +4278,8 @@
         <v>202</v>
       </c>
     </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A182" s="1">
+    <row r="182" spans="1:4">
+      <c r="A182" s="1" t="n">
         <v>1207</v>
       </c>
       <c r="B182" t="s">
@@ -4303,8 +4292,8 @@
         <v>204</v>
       </c>
     </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A183" s="1">
+    <row r="183" spans="1:4">
+      <c r="A183" s="1" t="n">
         <v>1208</v>
       </c>
       <c r="B183" t="s">
@@ -4317,8 +4306,8 @@
         <v>206</v>
       </c>
     </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A184" s="1">
+    <row r="184" spans="1:4">
+      <c r="A184" s="1" t="n">
         <v>1209</v>
       </c>
       <c r="B184" t="s">
@@ -4331,8 +4320,8 @@
         <v>208</v>
       </c>
     </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A185" s="1">
+    <row r="185" spans="1:4">
+      <c r="A185" s="1" t="n">
         <v>1210</v>
       </c>
       <c r="B185" t="s">
@@ -4345,8 +4334,8 @@
         <v>210</v>
       </c>
     </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A186" s="1">
+    <row r="186" spans="1:4">
+      <c r="A186" s="1" t="n">
         <v>1211</v>
       </c>
       <c r="B186" t="s">
@@ -4359,8 +4348,8 @@
         <v>211</v>
       </c>
     </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A187" s="1">
+    <row r="187" spans="1:4">
+      <c r="A187" s="1" t="n">
         <v>1212</v>
       </c>
       <c r="B187" t="s">
@@ -4373,8 +4362,8 @@
         <v>212</v>
       </c>
     </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A188" s="1">
+    <row r="188" spans="1:4">
+      <c r="A188" s="1" t="n">
         <v>1213</v>
       </c>
       <c r="B188" t="s">
@@ -4387,8 +4376,8 @@
         <v>213</v>
       </c>
     </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A189" s="1">
+    <row r="189" spans="1:4">
+      <c r="A189" s="1" t="n">
         <v>1214</v>
       </c>
       <c r="B189" t="s">
@@ -4401,8 +4390,8 @@
         <v>214</v>
       </c>
     </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A190" s="1">
+    <row r="190" spans="1:4">
+      <c r="A190" s="1" t="n">
         <v>1215</v>
       </c>
       <c r="B190" t="s">
@@ -4415,8 +4404,8 @@
         <v>216</v>
       </c>
     </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A191" s="1">
+    <row r="191" spans="1:4">
+      <c r="A191" s="1" t="n">
         <v>1216</v>
       </c>
       <c r="B191" t="s">
@@ -4429,8 +4418,8 @@
         <v>217</v>
       </c>
     </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A192" s="1">
+    <row r="192" spans="1:4">
+      <c r="A192" s="1" t="n">
         <v>1217</v>
       </c>
       <c r="B192" t="s">
@@ -4443,8 +4432,8 @@
         <v>219</v>
       </c>
     </row>
-    <row r="193" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A193" s="1">
+    <row r="193" spans="1:4">
+      <c r="A193" s="1" t="n">
         <v>1218</v>
       </c>
       <c r="B193" t="s">
@@ -4457,8 +4446,8 @@
         <v>220</v>
       </c>
     </row>
-    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A194" s="1">
+    <row r="194" spans="1:4">
+      <c r="A194" s="1" t="n">
         <v>1219</v>
       </c>
       <c r="B194" t="s">
@@ -4471,8 +4460,8 @@
         <v>222</v>
       </c>
     </row>
-    <row r="195" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A195" s="1">
+    <row r="195" spans="1:4">
+      <c r="A195" s="1" t="n">
         <v>1220</v>
       </c>
       <c r="B195" t="s">
@@ -4485,8 +4474,8 @@
         <v>208</v>
       </c>
     </row>
-    <row r="196" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A196" s="1">
+    <row r="196" spans="1:4">
+      <c r="A196" s="1" t="n">
         <v>1221</v>
       </c>
       <c r="B196" t="s">
@@ -4499,8 +4488,8 @@
         <v>210</v>
       </c>
     </row>
-    <row r="197" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A197" s="1">
+    <row r="197" spans="1:4">
+      <c r="A197" s="1" t="n">
         <v>1222</v>
       </c>
       <c r="B197" t="s">
@@ -4513,8 +4502,8 @@
         <v>224</v>
       </c>
     </row>
-    <row r="198" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A198" s="1">
+    <row r="198" spans="1:4">
+      <c r="A198" s="1" t="n">
         <v>1223</v>
       </c>
       <c r="B198" t="s">
@@ -4527,8 +4516,8 @@
         <v>217</v>
       </c>
     </row>
-    <row r="199" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A199" s="1">
+    <row r="199" spans="1:4">
+      <c r="A199" s="1" t="n">
         <v>1224</v>
       </c>
       <c r="B199" t="s">
@@ -4541,8 +4530,8 @@
         <v>219</v>
       </c>
     </row>
-    <row r="200" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A200" s="1">
+    <row r="200" spans="1:4">
+      <c r="A200" s="1" t="n">
         <v>1225</v>
       </c>
       <c r="B200" t="s">
@@ -4555,8 +4544,8 @@
         <v>220</v>
       </c>
     </row>
-    <row r="201" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A201" s="1">
+    <row r="201" spans="1:4">
+      <c r="A201" s="1" t="n">
         <v>1226</v>
       </c>
       <c r="B201" t="s">
@@ -4569,8 +4558,8 @@
         <v>226</v>
       </c>
     </row>
-    <row r="202" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A202" s="1">
+    <row r="202" spans="1:4">
+      <c r="A202" s="1" t="n">
         <v>1227</v>
       </c>
       <c r="B202" t="s">
@@ -4583,8 +4572,8 @@
         <v>227</v>
       </c>
     </row>
-    <row r="203" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A203" s="1">
+    <row r="203" spans="1:4">
+      <c r="A203" s="1" t="n">
         <v>1228</v>
       </c>
       <c r="B203" t="s">
@@ -4597,8 +4586,8 @@
         <v>228</v>
       </c>
     </row>
-    <row r="204" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A204" s="1">
+    <row r="204" spans="1:4">
+      <c r="A204" s="1" t="n">
         <v>1229</v>
       </c>
       <c r="B204" t="s">
@@ -4611,8 +4600,8 @@
         <v>230</v>
       </c>
     </row>
-    <row r="205" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A205" s="1">
+    <row r="205" spans="1:4">
+      <c r="A205" s="1" t="n">
         <v>1230</v>
       </c>
       <c r="B205" t="s">
@@ -4625,8 +4614,8 @@
         <v>231</v>
       </c>
     </row>
-    <row r="206" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A206" s="1">
+    <row r="206" spans="1:4">
+      <c r="A206" s="1" t="n">
         <v>1231</v>
       </c>
       <c r="B206" t="s">
@@ -4639,8 +4628,8 @@
         <v>233</v>
       </c>
     </row>
-    <row r="207" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A207" s="1">
+    <row r="207" spans="1:4">
+      <c r="A207" s="1" t="n">
         <v>1232</v>
       </c>
       <c r="B207" t="s">
@@ -4653,8 +4642,8 @@
         <v>234</v>
       </c>
     </row>
-    <row r="208" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A208" s="1">
+    <row r="208" spans="1:4">
+      <c r="A208" s="1" t="n">
         <v>1233</v>
       </c>
       <c r="B208" t="s">
@@ -4667,8 +4656,8 @@
         <v>235</v>
       </c>
     </row>
-    <row r="209" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A209" s="1">
+    <row r="209" spans="1:4">
+      <c r="A209" s="1" t="n">
         <v>1234</v>
       </c>
       <c r="B209" t="s">
@@ -4681,8 +4670,8 @@
         <v>236</v>
       </c>
     </row>
-    <row r="210" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A210" s="1">
+    <row r="210" spans="1:4">
+      <c r="A210" s="1" t="n">
         <v>1235</v>
       </c>
       <c r="B210" t="s">
@@ -4695,8 +4684,8 @@
         <v>211</v>
       </c>
     </row>
-    <row r="211" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A211" s="1">
+    <row r="211" spans="1:4">
+      <c r="A211" s="1" t="n">
         <v>1236</v>
       </c>
       <c r="B211" t="s">
@@ -4709,8 +4698,8 @@
         <v>212</v>
       </c>
     </row>
-    <row r="212" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A212" s="1">
+    <row r="212" spans="1:4">
+      <c r="A212" s="1" t="n">
         <v>1237</v>
       </c>
       <c r="B212" t="s">
@@ -4723,8 +4712,8 @@
         <v>237</v>
       </c>
     </row>
-    <row r="213" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A213" s="1">
+    <row r="213" spans="1:4">
+      <c r="A213" s="1" t="n">
         <v>1238</v>
       </c>
       <c r="B213" t="s">
@@ -4737,8 +4726,8 @@
         <v>239</v>
       </c>
     </row>
-    <row r="214" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A214" s="1">
+    <row r="214" spans="1:4">
+      <c r="A214" s="1" t="n">
         <v>1239</v>
       </c>
       <c r="B214" t="s">
@@ -4751,8 +4740,8 @@
         <v>242</v>
       </c>
     </row>
-    <row r="215" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A215" s="1">
+    <row r="215" spans="1:4">
+      <c r="A215" s="1" t="n">
         <v>1240</v>
       </c>
       <c r="B215" t="s">
@@ -4765,8 +4754,8 @@
         <v>243</v>
       </c>
     </row>
-    <row r="216" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A216" s="1">
+    <row r="216" spans="1:4">
+      <c r="A216" s="1" t="n">
         <v>1241</v>
       </c>
       <c r="B216" t="s">
@@ -4779,8 +4768,8 @@
         <v>244</v>
       </c>
     </row>
-    <row r="217" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A217" s="1">
+    <row r="217" spans="1:4">
+      <c r="A217" s="1" t="n">
         <v>1242</v>
       </c>
       <c r="B217" t="s">
@@ -4793,8 +4782,8 @@
         <v>245</v>
       </c>
     </row>
-    <row r="218" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A218" s="1">
+    <row r="218" spans="1:4">
+      <c r="A218" s="1" t="n">
         <v>1243</v>
       </c>
       <c r="B218" t="s">
@@ -4807,8 +4796,8 @@
         <v>246</v>
       </c>
     </row>
-    <row r="219" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A219" s="1">
+    <row r="219" spans="1:4">
+      <c r="A219" s="1" t="n">
         <v>1244</v>
       </c>
       <c r="B219" t="s">
@@ -4821,8 +4810,8 @@
         <v>247</v>
       </c>
     </row>
-    <row r="220" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A220" s="1">
+    <row r="220" spans="1:4">
+      <c r="A220" s="1" t="n">
         <v>1245</v>
       </c>
       <c r="B220" t="s">
@@ -4835,8 +4824,8 @@
         <v>250</v>
       </c>
     </row>
-    <row r="221" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A221" s="1">
+    <row r="221" spans="1:4">
+      <c r="A221" s="1" t="n">
         <v>1246</v>
       </c>
       <c r="B221" t="s">
@@ -4849,8 +4838,8 @@
         <v>252</v>
       </c>
     </row>
-    <row r="222" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A222" s="1">
+    <row r="222" spans="1:4">
+      <c r="A222" s="1" t="n">
         <v>1247</v>
       </c>
       <c r="B222" t="s">
@@ -4863,8 +4852,8 @@
         <v>255</v>
       </c>
     </row>
-    <row r="223" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A223" s="1">
+    <row r="223" spans="1:4">
+      <c r="A223" s="1" t="n">
         <v>1248</v>
       </c>
       <c r="B223" t="s">
@@ -4877,8 +4866,8 @@
         <v>258</v>
       </c>
     </row>
-    <row r="224" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A224" s="1">
+    <row r="224" spans="1:4">
+      <c r="A224" s="1" t="n">
         <v>1249</v>
       </c>
       <c r="B224" t="s">
@@ -4891,8 +4880,8 @@
         <v>259</v>
       </c>
     </row>
-    <row r="225" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A225" s="1">
+    <row r="225" spans="1:4">
+      <c r="A225" s="1" t="n">
         <v>1250</v>
       </c>
       <c r="B225" t="s">
@@ -4905,8 +4894,8 @@
         <v>262</v>
       </c>
     </row>
-    <row r="226" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A226" s="1">
+    <row r="226" spans="1:4">
+      <c r="A226" s="1" t="n">
         <v>1251</v>
       </c>
       <c r="B226" t="s">
@@ -4919,8 +4908,8 @@
         <v>265</v>
       </c>
     </row>
-    <row r="227" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A227" s="1">
+    <row r="227" spans="1:4">
+      <c r="A227" s="1" t="n">
         <v>1252</v>
       </c>
       <c r="B227" t="s">
@@ -4933,8 +4922,8 @@
         <v>268</v>
       </c>
     </row>
-    <row r="228" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A228" s="1">
+    <row r="228" spans="1:4">
+      <c r="A228" s="1" t="n">
         <v>1253</v>
       </c>
       <c r="B228" t="s">
@@ -4947,8 +4936,8 @@
         <v>271</v>
       </c>
     </row>
-    <row r="229" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A229" s="1">
+    <row r="229" spans="1:4">
+      <c r="A229" s="1" t="n">
         <v>1254</v>
       </c>
       <c r="B229" t="s">
@@ -4961,8 +4950,8 @@
         <v>274</v>
       </c>
     </row>
-    <row r="230" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A230" s="1">
+    <row r="230" spans="1:4">
+      <c r="A230" s="1" t="n">
         <v>1255</v>
       </c>
       <c r="B230" t="s">
@@ -4975,8 +4964,8 @@
         <v>277</v>
       </c>
     </row>
-    <row r="231" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A231" s="1">
+    <row r="231" spans="1:4">
+      <c r="A231" s="1" t="n">
         <v>1256</v>
       </c>
       <c r="B231" t="s">
@@ -4989,8 +4978,8 @@
         <v>279</v>
       </c>
     </row>
-    <row r="232" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A232" s="1">
+    <row r="232" spans="1:4">
+      <c r="A232" s="1" t="n">
         <v>1257</v>
       </c>
       <c r="B232" t="s">
@@ -5003,8 +4992,8 @@
         <v>282</v>
       </c>
     </row>
-    <row r="233" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A233" s="1">
+    <row r="233" spans="1:4">
+      <c r="A233" s="1" t="n">
         <v>1258</v>
       </c>
       <c r="B233" t="s">
@@ -5017,8 +5006,8 @@
         <v>285</v>
       </c>
     </row>
-    <row r="234" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A234" s="1">
+    <row r="234" spans="1:4">
+      <c r="A234" s="1" t="n">
         <v>1259</v>
       </c>
       <c r="B234" t="s">
@@ -5031,8 +5020,8 @@
         <v>288</v>
       </c>
     </row>
-    <row r="235" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A235" s="1">
+    <row r="235" spans="1:4">
+      <c r="A235" s="1" t="n">
         <v>1260</v>
       </c>
       <c r="B235" t="s">
@@ -5045,8 +5034,8 @@
         <v>291</v>
       </c>
     </row>
-    <row r="236" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A236" s="1">
+    <row r="236" spans="1:4">
+      <c r="A236" s="1" t="n">
         <v>1261</v>
       </c>
       <c r="B236" t="s">
@@ -5059,8 +5048,8 @@
         <v>294</v>
       </c>
     </row>
-    <row r="237" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A237" s="1">
+    <row r="237" spans="1:4">
+      <c r="A237" s="1" t="n">
         <v>1262</v>
       </c>
       <c r="B237" t="s">
@@ -5073,8 +5062,8 @@
         <v>296</v>
       </c>
     </row>
-    <row r="238" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A238" s="1">
+    <row r="238" spans="1:4">
+      <c r="A238" s="1" t="n">
         <v>1263</v>
       </c>
       <c r="B238" t="s">
@@ -5087,8 +5076,8 @@
         <v>299</v>
       </c>
     </row>
-    <row r="239" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A239" s="1">
+    <row r="239" spans="1:4">
+      <c r="A239" s="1" t="n">
         <v>1264</v>
       </c>
       <c r="B239" t="s">
@@ -5101,8 +5090,8 @@
         <v>302</v>
       </c>
     </row>
-    <row r="240" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A240" s="1">
+    <row r="240" spans="1:4">
+      <c r="A240" s="1" t="n">
         <v>1265</v>
       </c>
       <c r="B240" t="s">
@@ -5115,8 +5104,8 @@
         <v>305</v>
       </c>
     </row>
-    <row r="241" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A241" s="1">
+    <row r="241" spans="1:4">
+      <c r="A241" s="1" t="n">
         <v>1266</v>
       </c>
       <c r="B241" t="s">
@@ -5129,8 +5118,8 @@
         <v>308</v>
       </c>
     </row>
-    <row r="242" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A242" s="1">
+    <row r="242" spans="1:4">
+      <c r="A242" s="1" t="n">
         <v>1267</v>
       </c>
       <c r="B242" t="s">
@@ -5143,8 +5132,8 @@
         <v>311</v>
       </c>
     </row>
-    <row r="243" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A243" s="1">
+    <row r="243" spans="1:4">
+      <c r="A243" s="1" t="n">
         <v>1268</v>
       </c>
       <c r="B243" t="s">
@@ -5157,8 +5146,8 @@
         <v>314</v>
       </c>
     </row>
-    <row r="244" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A244" s="1">
+    <row r="244" spans="1:4">
+      <c r="A244" s="1" t="n">
         <v>1269</v>
       </c>
       <c r="B244" t="s">
@@ -5171,8 +5160,8 @@
         <v>317</v>
       </c>
     </row>
-    <row r="245" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A245" s="1">
+    <row r="245" spans="1:4">
+      <c r="A245" s="1" t="n">
         <v>1270</v>
       </c>
       <c r="B245" t="s">
@@ -5185,8 +5174,8 @@
         <v>320</v>
       </c>
     </row>
-    <row r="246" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A246" s="1">
+    <row r="246" spans="1:4">
+      <c r="A246" s="1" t="n">
         <v>1271</v>
       </c>
       <c r="B246" t="s">
@@ -5199,8 +5188,8 @@
         <v>323</v>
       </c>
     </row>
-    <row r="247" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A247" s="1">
+    <row r="247" spans="1:4">
+      <c r="A247" s="1" t="n">
         <v>1272</v>
       </c>
       <c r="B247" t="s">
@@ -5213,8 +5202,8 @@
         <v>325</v>
       </c>
     </row>
-    <row r="248" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A248" s="1">
+    <row r="248" spans="1:4">
+      <c r="A248" s="1" t="n">
         <v>1273</v>
       </c>
       <c r="B248" t="s">
@@ -5227,8 +5216,8 @@
         <v>327</v>
       </c>
     </row>
-    <row r="249" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A249" s="1">
+    <row r="249" spans="1:4">
+      <c r="A249" s="1" t="n">
         <v>1274</v>
       </c>
       <c r="B249" t="s">
@@ -5241,8 +5230,8 @@
         <v>329</v>
       </c>
     </row>
-    <row r="250" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A250" s="1">
+    <row r="250" spans="1:4">
+      <c r="A250" s="1" t="n">
         <v>1275</v>
       </c>
       <c r="B250" t="s">
@@ -5255,8 +5244,8 @@
         <v>331</v>
       </c>
     </row>
-    <row r="251" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A251" s="1">
+    <row r="251" spans="1:4">
+      <c r="A251" s="1" t="n">
         <v>1276</v>
       </c>
       <c r="B251" t="s">
@@ -5269,8 +5258,8 @@
         <v>333</v>
       </c>
     </row>
-    <row r="252" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A252" s="1">
+    <row r="252" spans="1:4">
+      <c r="A252" s="1" t="n">
         <v>1277</v>
       </c>
       <c r="B252" t="s">
@@ -5283,8 +5272,8 @@
         <v>335</v>
       </c>
     </row>
-    <row r="253" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A253" s="1">
+    <row r="253" spans="1:4">
+      <c r="A253" s="1" t="n">
         <v>1278</v>
       </c>
       <c r="B253" t="s">
@@ -5297,8 +5286,8 @@
         <v>337</v>
       </c>
     </row>
-    <row r="254" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A254" s="1">
+    <row r="254" spans="1:4">
+      <c r="A254" s="1" t="n">
         <v>1279</v>
       </c>
       <c r="B254" t="s">
@@ -5311,8 +5300,8 @@
         <v>339</v>
       </c>
     </row>
-    <row r="255" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A255" s="1">
+    <row r="255" spans="1:4">
+      <c r="A255" s="1" t="n">
         <v>1280</v>
       </c>
       <c r="B255" t="s">
@@ -5325,8 +5314,8 @@
         <v>341</v>
       </c>
     </row>
-    <row r="256" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A256" s="1">
+    <row r="256" spans="1:4">
+      <c r="A256" s="1" t="n">
         <v>1281</v>
       </c>
       <c r="B256" t="s">
@@ -5339,8 +5328,8 @@
         <v>343</v>
       </c>
     </row>
-    <row r="257" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A257" s="1">
+    <row r="257" spans="1:4">
+      <c r="A257" s="1" t="n">
         <v>1282</v>
       </c>
       <c r="B257" t="s">
@@ -5353,8 +5342,8 @@
         <v>345</v>
       </c>
     </row>
-    <row r="258" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A258" s="1">
+    <row r="258" spans="1:4">
+      <c r="A258" s="1" t="n">
         <v>1283</v>
       </c>
       <c r="B258" t="s">
@@ -5367,8 +5356,8 @@
         <v>347</v>
       </c>
     </row>
-    <row r="259" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A259" s="1">
+    <row r="259" spans="1:4">
+      <c r="A259" s="1" t="n">
         <v>1284</v>
       </c>
       <c r="B259" t="s">
@@ -5381,8 +5370,8 @@
         <v>349</v>
       </c>
     </row>
-    <row r="260" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A260" s="1">
+    <row r="260" spans="1:4">
+      <c r="A260" s="1" t="n">
         <v>1285</v>
       </c>
       <c r="B260" t="s">
@@ -5395,8 +5384,8 @@
         <v>351</v>
       </c>
     </row>
-    <row r="261" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A261" s="1">
+    <row r="261" spans="1:4">
+      <c r="A261" s="1" t="n">
         <v>1286</v>
       </c>
       <c r="B261" t="s">
@@ -5409,8 +5398,8 @@
         <v>353</v>
       </c>
     </row>
-    <row r="262" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A262" s="1">
+    <row r="262" spans="1:4">
+      <c r="A262" s="1" t="n">
         <v>1287</v>
       </c>
       <c r="B262" t="s">
@@ -5423,8 +5412,8 @@
         <v>355</v>
       </c>
     </row>
-    <row r="263" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A263" s="1">
+    <row r="263" spans="1:4">
+      <c r="A263" s="1" t="n">
         <v>1288</v>
       </c>
       <c r="B263" t="s">
@@ -5437,8 +5426,8 @@
         <v>356</v>
       </c>
     </row>
-    <row r="264" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A264" s="1">
+    <row r="264" spans="1:4">
+      <c r="A264" s="1" t="n">
         <v>1289</v>
       </c>
       <c r="B264" t="s">
@@ -5451,8 +5440,8 @@
         <v>358</v>
       </c>
     </row>
-    <row r="265" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A265" s="1">
+    <row r="265" spans="1:4">
+      <c r="A265" s="1" t="n">
         <v>1290</v>
       </c>
       <c r="B265" t="s">
@@ -5465,8 +5454,8 @@
         <v>359</v>
       </c>
     </row>
-    <row r="266" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A266" s="1">
+    <row r="266" spans="1:4">
+      <c r="A266" s="1" t="n">
         <v>1291</v>
       </c>
       <c r="B266" t="s">
@@ -5479,8 +5468,8 @@
         <v>361</v>
       </c>
     </row>
-    <row r="267" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A267" s="1">
+    <row r="267" spans="1:4">
+      <c r="A267" s="1" t="n">
         <v>1292</v>
       </c>
       <c r="B267" t="s">
@@ -5493,8 +5482,8 @@
         <v>363</v>
       </c>
     </row>
-    <row r="268" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A268" s="1">
+    <row r="268" spans="1:4">
+      <c r="A268" s="1" t="n">
         <v>1293</v>
       </c>
       <c r="B268" t="s">
@@ -5507,8 +5496,8 @@
         <v>364</v>
       </c>
     </row>
-    <row r="269" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A269" s="1">
+    <row r="269" spans="1:4">
+      <c r="A269" s="1" t="n">
         <v>1294</v>
       </c>
       <c r="B269" t="s">
@@ -5521,8 +5510,8 @@
         <v>365</v>
       </c>
     </row>
-    <row r="270" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A270" s="1">
+    <row r="270" spans="1:4">
+      <c r="A270" s="1" t="n">
         <v>1295</v>
       </c>
       <c r="B270" t="s">
@@ -5535,8 +5524,8 @@
         <v>366</v>
       </c>
     </row>
-    <row r="271" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A271" s="1">
+    <row r="271" spans="1:4">
+      <c r="A271" s="1" t="n">
         <v>1296</v>
       </c>
       <c r="B271" t="s">
@@ -5549,8 +5538,8 @@
         <v>363</v>
       </c>
     </row>
-    <row r="272" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A272" s="1">
+    <row r="272" spans="1:4">
+      <c r="A272" s="1" t="n">
         <v>1297</v>
       </c>
       <c r="B272" t="s">
@@ -5563,8 +5552,8 @@
         <v>363</v>
       </c>
     </row>
-    <row r="273" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A273" s="1">
+    <row r="273" spans="1:4">
+      <c r="A273" s="1" t="n">
         <v>1298</v>
       </c>
       <c r="B273" t="s">
@@ -5577,8 +5566,8 @@
         <v>363</v>
       </c>
     </row>
-    <row r="274" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A274" s="1">
+    <row r="274" spans="1:4">
+      <c r="A274" s="1" t="n">
         <v>1299</v>
       </c>
       <c r="B274" t="s">
@@ -5591,8 +5580,8 @@
         <v>363</v>
       </c>
     </row>
-    <row r="275" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A275" s="1">
+    <row r="275" spans="1:4">
+      <c r="A275" s="1" t="n">
         <v>1300</v>
       </c>
       <c r="B275" t="s">
@@ -5605,8 +5594,8 @@
         <v>363</v>
       </c>
     </row>
-    <row r="276" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A276" s="1">
+    <row r="276" spans="1:4">
+      <c r="A276" s="1" t="n">
         <v>1301</v>
       </c>
       <c r="B276" t="s">
@@ -5619,8 +5608,8 @@
         <v>366</v>
       </c>
     </row>
-    <row r="277" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A277" s="1">
+    <row r="277" spans="1:4">
+      <c r="A277" s="1" t="n">
         <v>1302</v>
       </c>
       <c r="B277" t="s">
@@ -5633,8 +5622,8 @@
         <v>366</v>
       </c>
     </row>
-    <row r="278" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A278" s="1">
+    <row r="278" spans="1:4">
+      <c r="A278" s="1" t="n">
         <v>1303</v>
       </c>
       <c r="B278" t="s">
@@ -5647,8 +5636,8 @@
         <v>366</v>
       </c>
     </row>
-    <row r="279" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A279" s="1">
+    <row r="279" spans="1:4">
+      <c r="A279" s="1" t="n">
         <v>1304</v>
       </c>
       <c r="B279" t="s">
@@ -5661,8 +5650,8 @@
         <v>368</v>
       </c>
     </row>
-    <row r="280" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A280" s="1">
+    <row r="280" spans="1:4">
+      <c r="A280" s="1" t="n">
         <v>1305</v>
       </c>
       <c r="B280" t="s">
@@ -5675,8 +5664,8 @@
         <v>369</v>
       </c>
     </row>
-    <row r="281" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A281" s="1">
+    <row r="281" spans="1:4">
+      <c r="A281" s="1" t="n">
         <v>1306</v>
       </c>
       <c r="B281" t="s">
@@ -5689,8 +5678,8 @@
         <v>371</v>
       </c>
     </row>
-    <row r="282" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A282" s="1">
+    <row r="282" spans="1:4">
+      <c r="A282" s="1" t="n">
         <v>1307</v>
       </c>
       <c r="B282" t="s">
@@ -5703,8 +5692,8 @@
         <v>373</v>
       </c>
     </row>
-    <row r="283" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A283" s="1">
+    <row r="283" spans="1:4">
+      <c r="A283" s="1" t="n">
         <v>1308</v>
       </c>
       <c r="B283" t="s">
@@ -5717,8 +5706,8 @@
         <v>375</v>
       </c>
     </row>
-    <row r="284" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A284" s="1">
+    <row r="284" spans="1:4">
+      <c r="A284" s="1" t="n">
         <v>1309</v>
       </c>
       <c r="B284" t="s">
@@ -5731,8 +5720,8 @@
         <v>377</v>
       </c>
     </row>
-    <row r="285" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A285" s="1">
+    <row r="285" spans="1:4">
+      <c r="A285" s="1" t="n">
         <v>1310</v>
       </c>
       <c r="B285" t="s">
@@ -5745,8 +5734,8 @@
         <v>369</v>
       </c>
     </row>
-    <row r="286" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A286" s="1">
+    <row r="286" spans="1:4">
+      <c r="A286" s="1" t="n">
         <v>1311</v>
       </c>
       <c r="B286" t="s">
@@ -5759,8 +5748,8 @@
         <v>380</v>
       </c>
     </row>
-    <row r="287" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A287" s="1">
+    <row r="287" spans="1:4">
+      <c r="A287" s="1" t="n">
         <v>1312</v>
       </c>
       <c r="B287" t="s">
@@ -5773,8 +5762,8 @@
         <v>368</v>
       </c>
     </row>
-    <row r="288" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A288" s="1">
+    <row r="288" spans="1:4">
+      <c r="A288" s="1" t="n">
         <v>1313</v>
       </c>
       <c r="B288" t="s">
@@ -5787,8 +5776,8 @@
         <v>368</v>
       </c>
     </row>
-    <row r="289" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A289" s="1">
+    <row r="289" spans="1:4">
+      <c r="A289" s="1" t="n">
         <v>1314</v>
       </c>
       <c r="B289" t="s">
@@ -5801,8 +5790,8 @@
         <v>383</v>
       </c>
     </row>
-    <row r="290" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A290" s="1">
+    <row r="290" spans="1:4">
+      <c r="A290" s="1" t="n">
         <v>1315</v>
       </c>
       <c r="B290" t="s">
@@ -5815,8 +5804,8 @@
         <v>385</v>
       </c>
     </row>
-    <row r="291" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A291" s="1">
+    <row r="291" spans="1:4">
+      <c r="A291" s="1" t="n">
         <v>1316</v>
       </c>
       <c r="B291" t="s">
@@ -5829,8 +5818,8 @@
         <v>387</v>
       </c>
     </row>
-    <row r="292" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A292" s="1">
+    <row r="292" spans="1:4">
+      <c r="A292" s="1" t="n">
         <v>1317</v>
       </c>
       <c r="B292" t="s">
@@ -5843,8 +5832,8 @@
         <v>388</v>
       </c>
     </row>
-    <row r="293" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A293" s="1">
+    <row r="293" spans="1:4">
+      <c r="A293" s="1" t="n">
         <v>1318</v>
       </c>
       <c r="B293" t="s">
@@ -5857,8 +5846,8 @@
         <v>371</v>
       </c>
     </row>
-    <row r="294" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A294" s="1">
+    <row r="294" spans="1:4">
+      <c r="A294" s="1" t="n">
         <v>1319</v>
       </c>
       <c r="B294" t="s">
@@ -5871,8 +5860,8 @@
         <v>373</v>
       </c>
     </row>
-    <row r="295" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A295" s="1">
+    <row r="295" spans="1:4">
+      <c r="A295" s="1" t="n">
         <v>1320</v>
       </c>
       <c r="B295" t="s">
@@ -5885,8 +5874,8 @@
         <v>392</v>
       </c>
     </row>
-    <row r="296" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A296" s="1">
+    <row r="296" spans="1:4">
+      <c r="A296" s="1" t="n">
         <v>1321</v>
       </c>
       <c r="B296" t="s">
@@ -5899,8 +5888,8 @@
         <v>394</v>
       </c>
     </row>
-    <row r="297" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A297" s="1">
+    <row r="297" spans="1:4">
+      <c r="A297" s="1" t="n">
         <v>1322</v>
       </c>
       <c r="B297" t="s">
@@ -5913,8 +5902,8 @@
         <v>394</v>
       </c>
     </row>
-    <row r="298" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A298" s="1">
+    <row r="298" spans="1:4">
+      <c r="A298" s="1" t="n">
         <v>1323</v>
       </c>
       <c r="B298" t="s">
@@ -5927,8 +5916,8 @@
         <v>397</v>
       </c>
     </row>
-    <row r="299" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A299" s="1">
+    <row r="299" spans="1:4">
+      <c r="A299" s="1" t="n">
         <v>1324</v>
       </c>
       <c r="B299" t="s">
@@ -5941,8 +5930,8 @@
         <v>397</v>
       </c>
     </row>
-    <row r="300" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A300" s="1">
+    <row r="300" spans="1:4">
+      <c r="A300" s="1" t="n">
         <v>1325</v>
       </c>
       <c r="B300" t="s">
@@ -5955,8 +5944,8 @@
         <v>397</v>
       </c>
     </row>
-    <row r="301" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A301" s="1">
+    <row r="301" spans="1:4">
+      <c r="A301" s="1" t="n">
         <v>1326</v>
       </c>
       <c r="B301" t="s">
@@ -5969,8 +5958,8 @@
         <v>397</v>
       </c>
     </row>
-    <row r="302" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A302" s="1">
+    <row r="302" spans="1:4">
+      <c r="A302" s="1" t="n">
         <v>1327</v>
       </c>
       <c r="B302" t="s">
@@ -5983,8 +5972,8 @@
         <v>400</v>
       </c>
     </row>
-    <row r="303" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A303" s="1">
+    <row r="303" spans="1:4">
+      <c r="A303" s="1" t="n">
         <v>1328</v>
       </c>
       <c r="B303" t="s">
@@ -5997,8 +5986,8 @@
         <v>400</v>
       </c>
     </row>
-    <row r="304" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A304" s="1">
+    <row r="304" spans="1:4">
+      <c r="A304" s="1" t="n">
         <v>1329</v>
       </c>
       <c r="B304" t="s">
@@ -6011,8 +6000,8 @@
         <v>401</v>
       </c>
     </row>
-    <row r="305" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A305" s="1">
+    <row r="305" spans="1:4">
+      <c r="A305" s="1" t="n">
         <v>1330</v>
       </c>
       <c r="B305" t="s">
@@ -6025,8 +6014,8 @@
         <v>403</v>
       </c>
     </row>
-    <row r="306" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A306" s="1">
+    <row r="306" spans="1:4">
+      <c r="A306" s="1" t="n">
         <v>1331</v>
       </c>
       <c r="B306" t="s">
@@ -6039,8 +6028,8 @@
         <v>405</v>
       </c>
     </row>
-    <row r="307" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A307" s="1">
+    <row r="307" spans="1:4">
+      <c r="A307" s="1" t="n">
         <v>1332</v>
       </c>
       <c r="B307" t="s">
@@ -6053,8 +6042,8 @@
         <v>405</v>
       </c>
     </row>
-    <row r="308" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A308" s="1">
+    <row r="308" spans="1:4">
+      <c r="A308" s="1" t="n">
         <v>1333</v>
       </c>
       <c r="B308" t="s">
@@ -6067,8 +6056,8 @@
         <v>406</v>
       </c>
     </row>
-    <row r="309" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A309" s="1">
+    <row r="309" spans="1:4">
+      <c r="A309" s="1" t="n">
         <v>1334</v>
       </c>
       <c r="B309" t="s">
@@ -6081,8 +6070,8 @@
         <v>406</v>
       </c>
     </row>
-    <row r="310" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A310" s="1">
+    <row r="310" spans="1:4">
+      <c r="A310" s="1" t="n">
         <v>1335</v>
       </c>
       <c r="B310" t="s">
@@ -6095,8 +6084,8 @@
         <v>407</v>
       </c>
     </row>
-    <row r="311" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A311" s="1">
+    <row r="311" spans="1:4">
+      <c r="A311" s="1" t="n">
         <v>1336</v>
       </c>
       <c r="B311" t="s">
@@ -6109,8 +6098,8 @@
         <v>407</v>
       </c>
     </row>
-    <row r="312" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A312" s="1">
+    <row r="312" spans="1:4">
+      <c r="A312" s="1" t="n">
         <v>1337</v>
       </c>
       <c r="B312" t="s">
@@ -6123,8 +6112,8 @@
         <v>407</v>
       </c>
     </row>
-    <row r="313" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A313" s="1">
+    <row r="313" spans="1:4">
+      <c r="A313" s="1" t="n">
         <v>1338</v>
       </c>
       <c r="B313" t="s">
@@ -6137,8 +6126,8 @@
         <v>410</v>
       </c>
     </row>
-    <row r="314" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A314" s="1">
+    <row r="314" spans="1:4">
+      <c r="A314" s="1" t="n">
         <v>1339</v>
       </c>
       <c r="B314" t="s">
@@ -6151,8 +6140,8 @@
         <v>410</v>
       </c>
     </row>
-    <row r="315" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A315" s="1">
+    <row r="315" spans="1:4">
+      <c r="A315" s="1" t="n">
         <v>1340</v>
       </c>
       <c r="B315" t="s">
@@ -6165,8 +6154,8 @@
         <v>410</v>
       </c>
     </row>
-    <row r="316" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A316" s="1">
+    <row r="316" spans="1:4">
+      <c r="A316" s="1" t="n">
         <v>1341</v>
       </c>
       <c r="B316" t="s">
@@ -6179,8 +6168,8 @@
         <v>412</v>
       </c>
     </row>
-    <row r="317" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A317" s="1">
+    <row r="317" spans="1:4">
+      <c r="A317" s="1" t="n">
         <v>1342</v>
       </c>
       <c r="B317" t="s">
@@ -6193,8 +6182,8 @@
         <v>414</v>
       </c>
     </row>
-    <row r="318" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A318" s="1">
+    <row r="318" spans="1:4">
+      <c r="A318" s="1" t="n">
         <v>1343</v>
       </c>
       <c r="B318" t="s">
@@ -6207,8 +6196,8 @@
         <v>416</v>
       </c>
     </row>
-    <row r="319" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A319" s="1">
+    <row r="319" spans="1:4">
+      <c r="A319" s="1" t="n">
         <v>1344</v>
       </c>
       <c r="B319" t="s">
@@ -6221,8 +6210,8 @@
         <v>417</v>
       </c>
     </row>
-    <row r="320" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A320" s="1">
+    <row r="320" spans="1:4">
+      <c r="A320" s="1" t="n">
         <v>1345</v>
       </c>
       <c r="B320" t="s">
@@ -6235,8 +6224,8 @@
         <v>418</v>
       </c>
     </row>
-    <row r="321" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A321" s="1">
+    <row r="321" spans="1:4">
+      <c r="A321" s="1" t="n">
         <v>1346</v>
       </c>
       <c r="B321" t="s">
@@ -6249,8 +6238,8 @@
         <v>420</v>
       </c>
     </row>
-    <row r="322" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A322" s="1">
+    <row r="322" spans="1:4">
+      <c r="A322" s="1" t="n">
         <v>1347</v>
       </c>
       <c r="B322" t="s">
@@ -6263,8 +6252,8 @@
         <v>421</v>
       </c>
     </row>
-    <row r="323" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A323" s="1">
+    <row r="323" spans="1:4">
+      <c r="A323" s="1" t="n">
         <v>1348</v>
       </c>
       <c r="B323" t="s">
@@ -6277,8 +6266,8 @@
         <v>421</v>
       </c>
     </row>
-    <row r="324" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A324" s="1">
+    <row r="324" spans="1:4">
+      <c r="A324" s="1" t="n">
         <v>1349</v>
       </c>
       <c r="B324" t="s">
@@ -6291,8 +6280,8 @@
         <v>423</v>
       </c>
     </row>
-    <row r="325" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A325" s="1">
+    <row r="325" spans="1:4">
+      <c r="A325" s="1" t="n">
         <v>1350</v>
       </c>
       <c r="B325" t="s">
@@ -6305,8 +6294,8 @@
         <v>423</v>
       </c>
     </row>
-    <row r="326" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A326" s="1">
+    <row r="326" spans="1:4">
+      <c r="A326" s="1" t="n">
         <v>1351</v>
       </c>
       <c r="B326" t="s">
@@ -6319,8 +6308,8 @@
         <v>423</v>
       </c>
     </row>
-    <row r="327" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A327" s="1">
+    <row r="327" spans="1:4">
+      <c r="A327" s="1" t="n">
         <v>1352</v>
       </c>
       <c r="B327" t="s">
@@ -6333,8 +6322,8 @@
         <v>423</v>
       </c>
     </row>
-    <row r="328" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A328" s="1">
+    <row r="328" spans="1:4">
+      <c r="A328" s="1" t="n">
         <v>1353</v>
       </c>
       <c r="B328" t="s">
@@ -6347,8 +6336,8 @@
         <v>423</v>
       </c>
     </row>
-    <row r="329" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A329" s="1">
+    <row r="329" spans="1:4">
+      <c r="A329" s="1" t="n">
         <v>1354</v>
       </c>
       <c r="B329" t="s">
@@ -6361,8 +6350,8 @@
         <v>423</v>
       </c>
     </row>
-    <row r="330" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A330" s="1">
+    <row r="330" spans="1:4">
+      <c r="A330" s="1" t="n">
         <v>1355</v>
       </c>
       <c r="B330" t="s">
@@ -6375,8 +6364,8 @@
         <v>423</v>
       </c>
     </row>
-    <row r="331" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A331" s="1">
+    <row r="331" spans="1:4">
+      <c r="A331" s="1" t="n">
         <v>1356</v>
       </c>
       <c r="B331" t="s">
@@ -6389,8 +6378,8 @@
         <v>432</v>
       </c>
     </row>
-    <row r="332" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A332" s="1">
+    <row r="332" spans="1:4">
+      <c r="A332" s="1" t="n">
         <v>1357</v>
       </c>
       <c r="B332" t="s">
@@ -6403,8 +6392,8 @@
         <v>434</v>
       </c>
     </row>
-    <row r="333" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A333" s="1">
+    <row r="333" spans="1:4">
+      <c r="A333" s="1" t="n">
         <v>1358</v>
       </c>
       <c r="B333" t="s">
@@ -6417,8 +6406,8 @@
         <v>436</v>
       </c>
     </row>
-    <row r="334" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A334" s="1">
+    <row r="334" spans="1:4">
+      <c r="A334" s="1" t="n">
         <v>1359</v>
       </c>
       <c r="B334" t="s">
@@ -6431,8 +6420,8 @@
         <v>438</v>
       </c>
     </row>
-    <row r="335" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A335" s="1">
+    <row r="335" spans="1:4">
+      <c r="A335" s="1" t="n">
         <v>1360</v>
       </c>
       <c r="B335" t="s">
@@ -6445,8 +6434,8 @@
         <v>440</v>
       </c>
     </row>
-    <row r="336" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A336" s="1">
+    <row r="336" spans="1:4">
+      <c r="A336" s="1" t="n">
         <v>1361</v>
       </c>
       <c r="B336" t="s">
@@ -6459,8 +6448,8 @@
         <v>432</v>
       </c>
     </row>
-    <row r="337" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A337" s="1">
+    <row r="337" spans="1:4">
+      <c r="A337" s="1" t="n">
         <v>1362</v>
       </c>
       <c r="B337" t="s">
@@ -6473,8 +6462,8 @@
         <v>434</v>
       </c>
     </row>
-    <row r="338" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A338" s="1">
+    <row r="338" spans="1:4">
+      <c r="A338" s="1" t="n">
         <v>1363</v>
       </c>
       <c r="B338" t="s">
@@ -6487,8 +6476,8 @@
         <v>436</v>
       </c>
     </row>
-    <row r="339" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A339" s="1">
+    <row r="339" spans="1:4">
+      <c r="A339" s="1" t="n">
         <v>1364</v>
       </c>
       <c r="B339" t="s">
@@ -6501,8 +6490,8 @@
         <v>438</v>
       </c>
     </row>
-    <row r="340" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A340" s="1">
+    <row r="340" spans="1:4">
+      <c r="A340" s="1" t="n">
         <v>1365</v>
       </c>
       <c r="B340" t="s">
@@ -6515,8 +6504,8 @@
         <v>440</v>
       </c>
     </row>
-    <row r="341" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A341" s="1">
+    <row r="341" spans="1:4">
+      <c r="A341" s="1" t="n">
         <v>1366</v>
       </c>
       <c r="B341" t="s">
@@ -6529,8 +6518,8 @@
         <v>432</v>
       </c>
     </row>
-    <row r="342" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A342" s="1">
+    <row r="342" spans="1:4">
+      <c r="A342" s="1" t="n">
         <v>1367</v>
       </c>
       <c r="B342" t="s">
@@ -6543,8 +6532,8 @@
         <v>434</v>
       </c>
     </row>
-    <row r="343" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A343" s="1">
+    <row r="343" spans="1:4">
+      <c r="A343" s="1" t="n">
         <v>1368</v>
       </c>
       <c r="B343" t="s">
@@ -6557,8 +6546,8 @@
         <v>436</v>
       </c>
     </row>
-    <row r="344" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A344" s="1">
+    <row r="344" spans="1:4">
+      <c r="A344" s="1" t="n">
         <v>1369</v>
       </c>
       <c r="B344" t="s">
@@ -6571,8 +6560,8 @@
         <v>438</v>
       </c>
     </row>
-    <row r="345" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A345" s="1">
+    <row r="345" spans="1:4">
+      <c r="A345" s="1" t="n">
         <v>1370</v>
       </c>
       <c r="B345" t="s">
@@ -6585,8 +6574,8 @@
         <v>440</v>
       </c>
     </row>
-    <row r="346" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A346" s="1">
+    <row r="346" spans="1:4">
+      <c r="A346" s="1" t="n">
         <v>1623</v>
       </c>
       <c r="B346" t="s">
@@ -6599,8 +6588,8 @@
         <v>441</v>
       </c>
     </row>
-    <row r="347" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A347" s="1">
+    <row r="347" spans="1:4">
+      <c r="A347" s="1" t="n">
         <v>1624</v>
       </c>
       <c r="B347" t="s">
@@ -6613,8 +6602,8 @@
         <v>442</v>
       </c>
     </row>
-    <row r="348" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A348" s="1">
+    <row r="348" spans="1:4">
+      <c r="A348" s="1" t="n">
         <v>1625</v>
       </c>
       <c r="B348" t="s">
@@ -6627,8 +6616,8 @@
         <v>443</v>
       </c>
     </row>
-    <row r="349" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A349" s="1">
+    <row r="349" spans="1:4">
+      <c r="A349" s="1" t="n">
         <v>1626</v>
       </c>
       <c r="B349" t="s">
@@ -6641,8 +6630,8 @@
         <v>444</v>
       </c>
     </row>
-    <row r="350" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A350" s="1">
+    <row r="350" spans="1:4">
+      <c r="A350" s="1" t="n">
         <v>1627</v>
       </c>
       <c r="B350" t="s">
@@ -6655,8 +6644,8 @@
         <v>445</v>
       </c>
     </row>
-    <row r="351" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A351" s="1">
+    <row r="351" spans="1:4">
+      <c r="A351" s="1" t="n">
         <v>1628</v>
       </c>
       <c r="B351" t="s">
@@ -6669,8 +6658,8 @@
         <v>446</v>
       </c>
     </row>
-    <row r="352" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A352" s="1">
+    <row r="352" spans="1:4">
+      <c r="A352" s="1" t="n">
         <v>1629</v>
       </c>
       <c r="B352" t="s">
@@ -6683,8 +6672,8 @@
         <v>447</v>
       </c>
     </row>
-    <row r="353" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A353" s="1">
+    <row r="353" spans="1:4">
+      <c r="A353" s="1" t="n">
         <v>1630</v>
       </c>
       <c r="B353" t="s">
@@ -6697,8 +6686,8 @@
         <v>448</v>
       </c>
     </row>
-    <row r="354" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A354" s="1">
+    <row r="354" spans="1:4">
+      <c r="A354" s="1" t="n">
         <v>1631</v>
       </c>
       <c r="B354" t="s">
@@ -6711,8 +6700,8 @@
         <v>445</v>
       </c>
     </row>
-    <row r="355" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A355" s="1">
+    <row r="355" spans="1:4">
+      <c r="A355" s="1" t="n">
         <v>1632</v>
       </c>
       <c r="B355" t="s">
@@ -6725,8 +6714,8 @@
         <v>449</v>
       </c>
     </row>
-    <row r="356" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A356" s="1">
+    <row r="356" spans="1:4">
+      <c r="A356" s="1" t="n">
         <v>1633</v>
       </c>
       <c r="B356" t="s">
@@ -6739,8 +6728,8 @@
         <v>450</v>
       </c>
     </row>
-    <row r="357" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A357" s="1">
+    <row r="357" spans="1:4">
+      <c r="A357" s="1" t="n">
         <v>1634</v>
       </c>
       <c r="B357" t="s">
@@ -6753,8 +6742,8 @@
         <v>450</v>
       </c>
     </row>
-    <row r="358" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A358" s="1">
+    <row r="358" spans="1:4">
+      <c r="A358" s="1" t="n">
         <v>1635</v>
       </c>
       <c r="B358" t="s">
@@ -6767,8 +6756,8 @@
         <v>451</v>
       </c>
     </row>
-    <row r="359" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A359" s="1">
+    <row r="359" spans="1:4">
+      <c r="A359" s="1" t="n">
         <v>1636</v>
       </c>
       <c r="B359" t="s">
@@ -6781,8 +6770,8 @@
         <v>451</v>
       </c>
     </row>
-    <row r="360" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A360" s="1">
+    <row r="360" spans="1:4">
+      <c r="A360" s="1" t="n">
         <v>1637</v>
       </c>
       <c r="B360" t="s">
@@ -6795,8 +6784,8 @@
         <v>451</v>
       </c>
     </row>
-    <row r="361" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A361" s="1">
+    <row r="361" spans="1:4">
+      <c r="A361" s="1" t="n">
         <v>1638</v>
       </c>
       <c r="B361" t="s">
@@ -6809,8 +6798,8 @@
         <v>452</v>
       </c>
     </row>
-    <row r="362" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A362" s="1">
+    <row r="362" spans="1:4">
+      <c r="A362" s="1" t="n">
         <v>1639</v>
       </c>
       <c r="B362" t="s">
@@ -6823,8 +6812,8 @@
         <v>453</v>
       </c>
     </row>
-    <row r="363" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A363" s="1">
+    <row r="363" spans="1:4">
+      <c r="A363" s="1" t="n">
         <v>1640</v>
       </c>
       <c r="B363" t="s">
@@ -6837,8 +6826,8 @@
         <v>454</v>
       </c>
     </row>
-    <row r="364" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A364" s="1">
+    <row r="364" spans="1:4">
+      <c r="A364" s="1" t="n">
         <v>1641</v>
       </c>
       <c r="B364" t="s">
@@ -6851,8 +6840,8 @@
         <v>455</v>
       </c>
     </row>
-    <row r="365" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A365" s="1">
+    <row r="365" spans="1:4">
+      <c r="A365" s="1" t="n">
         <v>1642</v>
       </c>
       <c r="B365" t="s">
@@ -6865,8 +6854,8 @@
         <v>456</v>
       </c>
     </row>
-    <row r="366" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A366" s="1">
+    <row r="366" spans="1:4">
+      <c r="A366" s="1" t="n">
         <v>1643</v>
       </c>
       <c r="B366" t="s">
@@ -6879,8 +6868,8 @@
         <v>457</v>
       </c>
     </row>
-    <row r="367" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A367" s="1">
+    <row r="367" spans="1:4">
+      <c r="A367" s="1" t="n">
         <v>1644</v>
       </c>
       <c r="B367" t="s">
@@ -6893,8 +6882,8 @@
         <v>441</v>
       </c>
     </row>
-    <row r="368" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A368" s="1">
+    <row r="368" spans="1:4">
+      <c r="A368" s="1" t="n">
         <v>1645</v>
       </c>
       <c r="B368" t="s">
@@ -6907,8 +6896,8 @@
         <v>442</v>
       </c>
     </row>
-    <row r="369" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A369" s="1">
+    <row r="369" spans="1:4">
+      <c r="A369" s="1" t="n">
         <v>1646</v>
       </c>
       <c r="B369" t="s">
@@ -6921,8 +6910,8 @@
         <v>443</v>
       </c>
     </row>
-    <row r="370" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A370" s="1">
+    <row r="370" spans="1:4">
+      <c r="A370" s="1" t="n">
         <v>1647</v>
       </c>
       <c r="B370" t="s">
@@ -6935,8 +6924,8 @@
         <v>444</v>
       </c>
     </row>
-    <row r="371" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A371" s="1">
+    <row r="371" spans="1:4">
+      <c r="A371" s="1" t="n">
         <v>1648</v>
       </c>
       <c r="B371" t="s">
@@ -6949,8 +6938,8 @@
         <v>445</v>
       </c>
     </row>
-    <row r="372" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A372" s="1">
+    <row r="372" spans="1:4">
+      <c r="A372" s="1" t="n">
         <v>1649</v>
       </c>
       <c r="B372" t="s">
@@ -6963,8 +6952,8 @@
         <v>446</v>
       </c>
     </row>
-    <row r="373" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A373" s="1">
+    <row r="373" spans="1:4">
+      <c r="A373" s="1" t="n">
         <v>1650</v>
       </c>
       <c r="B373" t="s">
@@ -6977,8 +6966,8 @@
         <v>447</v>
       </c>
     </row>
-    <row r="374" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A374" s="1">
+    <row r="374" spans="1:4">
+      <c r="A374" s="1" t="n">
         <v>1651</v>
       </c>
       <c r="B374" t="s">
@@ -6991,8 +6980,8 @@
         <v>448</v>
       </c>
     </row>
-    <row r="375" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A375" s="1">
+    <row r="375" spans="1:4">
+      <c r="A375" s="1" t="n">
         <v>1652</v>
       </c>
       <c r="B375" t="s">
@@ -7005,8 +6994,8 @@
         <v>445</v>
       </c>
     </row>
-    <row r="376" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A376" s="1">
+    <row r="376" spans="1:4">
+      <c r="A376" s="1" t="n">
         <v>1653</v>
       </c>
       <c r="B376" t="s">
@@ -7019,8 +7008,8 @@
         <v>449</v>
       </c>
     </row>
-    <row r="377" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A377" s="1">
+    <row r="377" spans="1:4">
+      <c r="A377" s="1" t="n">
         <v>1654</v>
       </c>
       <c r="B377" t="s">
@@ -7033,8 +7022,8 @@
         <v>450</v>
       </c>
     </row>
-    <row r="378" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A378" s="1">
+    <row r="378" spans="1:4">
+      <c r="A378" s="1" t="n">
         <v>1655</v>
       </c>
       <c r="B378" t="s">
@@ -7047,8 +7036,8 @@
         <v>450</v>
       </c>
     </row>
-    <row r="379" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A379" s="1">
+    <row r="379" spans="1:4">
+      <c r="A379" s="1" t="n">
         <v>1656</v>
       </c>
       <c r="B379" t="s">
@@ -7061,8 +7050,8 @@
         <v>451</v>
       </c>
     </row>
-    <row r="380" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A380" s="1">
+    <row r="380" spans="1:4">
+      <c r="A380" s="1" t="n">
         <v>1657</v>
       </c>
       <c r="B380" t="s">
@@ -7075,8 +7064,8 @@
         <v>451</v>
       </c>
     </row>
-    <row r="381" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A381" s="1">
+    <row r="381" spans="1:4">
+      <c r="A381" s="1" t="n">
         <v>1658</v>
       </c>
       <c r="B381" t="s">
@@ -7089,8 +7078,8 @@
         <v>451</v>
       </c>
     </row>
-    <row r="382" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A382" s="1">
+    <row r="382" spans="1:4">
+      <c r="A382" s="1" t="n">
         <v>1659</v>
       </c>
       <c r="B382" t="s">
@@ -7103,8 +7092,8 @@
         <v>452</v>
       </c>
     </row>
-    <row r="383" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A383" s="1">
+    <row r="383" spans="1:4">
+      <c r="A383" s="1" t="n">
         <v>1660</v>
       </c>
       <c r="B383" t="s">
@@ -7117,8 +7106,8 @@
         <v>453</v>
       </c>
     </row>
-    <row r="384" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A384" s="1">
+    <row r="384" spans="1:4">
+      <c r="A384" s="1" t="n">
         <v>1661</v>
       </c>
       <c r="B384" t="s">
@@ -7131,8 +7120,8 @@
         <v>454</v>
       </c>
     </row>
-    <row r="385" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A385" s="1">
+    <row r="385" spans="1:4">
+      <c r="A385" s="1" t="n">
         <v>1662</v>
       </c>
       <c r="B385" t="s">
@@ -7145,8 +7134,8 @@
         <v>455</v>
       </c>
     </row>
-    <row r="386" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A386" s="1">
+    <row r="386" spans="1:4">
+      <c r="A386" s="1" t="n">
         <v>1663</v>
       </c>
       <c r="B386" t="s">
@@ -7159,8 +7148,8 @@
         <v>456</v>
       </c>
     </row>
-    <row r="387" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A387" s="1">
+    <row r="387" spans="1:4">
+      <c r="A387" s="1" t="n">
         <v>1664</v>
       </c>
       <c r="B387" t="s">
@@ -7173,8 +7162,8 @@
         <v>457</v>
       </c>
     </row>
-    <row r="388" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A388" s="1">
+    <row r="388" spans="1:4">
+      <c r="A388" s="1" t="n">
         <v>1665</v>
       </c>
       <c r="B388" t="s">
@@ -7187,8 +7176,8 @@
         <v>441</v>
       </c>
     </row>
-    <row r="389" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A389" s="1">
+    <row r="389" spans="1:4">
+      <c r="A389" s="1" t="n">
         <v>1666</v>
       </c>
       <c r="B389" t="s">
@@ -7201,8 +7190,8 @@
         <v>442</v>
       </c>
     </row>
-    <row r="390" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A390" s="1">
+    <row r="390" spans="1:4">
+      <c r="A390" s="1" t="n">
         <v>1667</v>
       </c>
       <c r="B390" t="s">
@@ -7215,8 +7204,8 @@
         <v>443</v>
       </c>
     </row>
-    <row r="391" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A391" s="1">
+    <row r="391" spans="1:4">
+      <c r="A391" s="1" t="n">
         <v>1668</v>
       </c>
       <c r="B391" t="s">
@@ -7229,8 +7218,8 @@
         <v>444</v>
       </c>
     </row>
-    <row r="392" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A392" s="1">
+    <row r="392" spans="1:4">
+      <c r="A392" s="1" t="n">
         <v>1669</v>
       </c>
       <c r="B392" t="s">
@@ -7243,8 +7232,8 @@
         <v>445</v>
       </c>
     </row>
-    <row r="393" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A393" s="1">
+    <row r="393" spans="1:4">
+      <c r="A393" s="1" t="n">
         <v>1670</v>
       </c>
       <c r="B393" t="s">
@@ -7257,8 +7246,8 @@
         <v>446</v>
       </c>
     </row>
-    <row r="394" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A394" s="1">
+    <row r="394" spans="1:4">
+      <c r="A394" s="1" t="n">
         <v>1671</v>
       </c>
       <c r="B394" t="s">
@@ -7271,8 +7260,8 @@
         <v>447</v>
       </c>
     </row>
-    <row r="395" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A395" s="1">
+    <row r="395" spans="1:4">
+      <c r="A395" s="1" t="n">
         <v>1672</v>
       </c>
       <c r="B395" t="s">
@@ -7285,8 +7274,8 @@
         <v>448</v>
       </c>
     </row>
-    <row r="396" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A396" s="1">
+    <row r="396" spans="1:4">
+      <c r="A396" s="1" t="n">
         <v>1673</v>
       </c>
       <c r="B396" t="s">
@@ -7299,8 +7288,8 @@
         <v>445</v>
       </c>
     </row>
-    <row r="397" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A397" s="1">
+    <row r="397" spans="1:4">
+      <c r="A397" s="1" t="n">
         <v>1674</v>
       </c>
       <c r="B397" t="s">
@@ -7313,8 +7302,8 @@
         <v>449</v>
       </c>
     </row>
-    <row r="398" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A398" s="1">
+    <row r="398" spans="1:4">
+      <c r="A398" s="1" t="n">
         <v>1675</v>
       </c>
       <c r="B398" t="s">
@@ -7327,8 +7316,8 @@
         <v>450</v>
       </c>
     </row>
-    <row r="399" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A399" s="1">
+    <row r="399" spans="1:4">
+      <c r="A399" s="1" t="n">
         <v>1676</v>
       </c>
       <c r="B399" t="s">
@@ -7341,8 +7330,8 @@
         <v>450</v>
       </c>
     </row>
-    <row r="400" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A400" s="1">
+    <row r="400" spans="1:4">
+      <c r="A400" s="1" t="n">
         <v>1677</v>
       </c>
       <c r="B400" t="s">
@@ -7355,8 +7344,8 @@
         <v>451</v>
       </c>
     </row>
-    <row r="401" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A401" s="1">
+    <row r="401" spans="1:4">
+      <c r="A401" s="1" t="n">
         <v>1678</v>
       </c>
       <c r="B401" t="s">
@@ -7369,8 +7358,8 @@
         <v>451</v>
       </c>
     </row>
-    <row r="402" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A402" s="1">
+    <row r="402" spans="1:4">
+      <c r="A402" s="1" t="n">
         <v>1679</v>
       </c>
       <c r="B402" t="s">
@@ -7383,8 +7372,8 @@
         <v>451</v>
       </c>
     </row>
-    <row r="403" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A403" s="1">
+    <row r="403" spans="1:4">
+      <c r="A403" s="1" t="n">
         <v>1680</v>
       </c>
       <c r="B403" t="s">
@@ -7397,8 +7386,8 @@
         <v>452</v>
       </c>
     </row>
-    <row r="404" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A404" s="1">
+    <row r="404" spans="1:4">
+      <c r="A404" s="1" t="n">
         <v>1681</v>
       </c>
       <c r="B404" t="s">
@@ -7411,8 +7400,8 @@
         <v>453</v>
       </c>
     </row>
-    <row r="405" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A405" s="1">
+    <row r="405" spans="1:4">
+      <c r="A405" s="1" t="n">
         <v>1682</v>
       </c>
       <c r="B405" t="s">
@@ -7425,8 +7414,8 @@
         <v>454</v>
       </c>
     </row>
-    <row r="406" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A406" s="1">
+    <row r="406" spans="1:4">
+      <c r="A406" s="1" t="n">
         <v>1683</v>
       </c>
       <c r="B406" t="s">
@@ -7439,8 +7428,8 @@
         <v>455</v>
       </c>
     </row>
-    <row r="407" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A407" s="1">
+    <row r="407" spans="1:4">
+      <c r="A407" s="1" t="n">
         <v>1684</v>
       </c>
       <c r="B407" t="s">
@@ -7453,8 +7442,8 @@
         <v>456</v>
       </c>
     </row>
-    <row r="408" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A408" s="1">
+    <row r="408" spans="1:4">
+      <c r="A408" s="1" t="n">
         <v>1685</v>
       </c>
       <c r="B408" t="s">
@@ -7468,6 +7457,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>